<commit_message>
Agregado de estado "terminado" scrum.xlsx y agregado de unos graficos en TESIS FINAL 3.25.docx
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="138">
   <si>
     <t>Product Backlog Items-Prototipo de Realidad Aumentada</t>
   </si>
@@ -903,6 +903,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -912,18 +927,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -947,38 +979,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1290,13 +1290,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="41"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="46"/>
     </row>
     <row r="2" spans="1:5" ht="30.75" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -1571,65 +1571,65 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A20" s="56">
+      <c r="A20" s="39">
         <v>17</v>
       </c>
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57">
+      <c r="C20" s="40"/>
+      <c r="D20" s="40">
         <v>10</v>
       </c>
-      <c r="E20" s="57" t="s">
+      <c r="E20" s="40" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A21" s="56">
+      <c r="A21" s="39">
         <v>18</v>
       </c>
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57">
+      <c r="C21" s="40"/>
+      <c r="D21" s="40">
         <v>3</v>
       </c>
-      <c r="E21" s="57" t="s">
+      <c r="E21" s="40" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A22" s="56">
+      <c r="A22" s="39">
         <v>19</v>
       </c>
-      <c r="B22" s="57" t="s">
+      <c r="B22" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57">
+      <c r="C22" s="40"/>
+      <c r="D22" s="40">
         <v>10</v>
       </c>
-      <c r="E22" s="57"/>
+      <c r="E22" s="40"/>
     </row>
     <row r="23" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A23" s="56">
+      <c r="A23" s="39">
         <v>20</v>
       </c>
-      <c r="B23" s="57" t="s">
+      <c r="B23" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57">
+      <c r="C23" s="40"/>
+      <c r="D23" s="40">
         <v>13</v>
       </c>
-      <c r="E23" s="57" t="s">
+      <c r="E23" s="40" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A24" s="56">
+      <c r="A24" s="39">
         <v>21</v>
       </c>
       <c r="B24" s="36" t="s">
@@ -1644,7 +1644,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A25" s="56">
+      <c r="A25" s="39">
         <v>22</v>
       </c>
       <c r="B25" s="36" t="s">
@@ -1661,7 +1661,7 @@
       <c r="G25" s="29"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A26" s="56">
+      <c r="A26" s="39">
         <v>23</v>
       </c>
       <c r="B26" s="36" t="s">
@@ -1676,7 +1676,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A27" s="56">
+      <c r="A27" s="39">
         <v>24</v>
       </c>
       <c r="B27" s="36" t="s">
@@ -1691,7 +1691,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A28" s="56">
+      <c r="A28" s="39">
         <v>25</v>
       </c>
       <c r="B28" s="36" t="s">
@@ -1706,7 +1706,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A29" s="56">
+      <c r="A29" s="39">
         <v>26</v>
       </c>
       <c r="B29" s="36" t="s">
@@ -1721,7 +1721,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A30" s="56">
+      <c r="A30" s="39">
         <v>27</v>
       </c>
       <c r="B30" s="36" t="s">
@@ -1736,7 +1736,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A31" s="56">
+      <c r="A31" s="39">
         <v>28</v>
       </c>
       <c r="B31" s="36" t="s">
@@ -1751,7 +1751,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A32" s="56">
+      <c r="A32" s="39">
         <v>29</v>
       </c>
       <c r="B32" s="32" t="s">
@@ -1766,7 +1766,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A33" s="56">
+      <c r="A33" s="39">
         <v>30</v>
       </c>
       <c r="B33" s="36" t="s">
@@ -1781,7 +1781,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A34" s="56">
+      <c r="A34" s="39">
         <v>31</v>
       </c>
       <c r="B34" s="38" t="s">
@@ -1796,7 +1796,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A35" s="56">
+      <c r="A35" s="39">
         <v>32</v>
       </c>
       <c r="B35" s="36" t="s">
@@ -1811,7 +1811,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A36" s="56">
+      <c r="A36" s="39">
         <v>33</v>
       </c>
       <c r="B36" s="36" t="s">
@@ -1826,7 +1826,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A37" s="56">
+      <c r="A37" s="39">
         <v>34</v>
       </c>
       <c r="B37" s="36" t="s">
@@ -1841,7 +1841,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A38" s="56">
+      <c r="A38" s="39">
         <v>35</v>
       </c>
       <c r="B38" s="36" t="s">
@@ -1856,7 +1856,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A39" s="56">
+      <c r="A39" s="39">
         <v>36</v>
       </c>
       <c r="B39" s="36" t="s">
@@ -1871,172 +1871,172 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A40" s="56">
+      <c r="A40" s="39">
         <v>37</v>
       </c>
-      <c r="B40" s="57" t="s">
+      <c r="B40" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="57"/>
-      <c r="D40" s="57">
+      <c r="C40" s="40"/>
+      <c r="D40" s="40">
         <v>7</v>
       </c>
-      <c r="E40" s="57" t="s">
+      <c r="E40" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A41" s="56">
+      <c r="A41" s="39">
         <v>38</v>
       </c>
-      <c r="B41" s="57" t="s">
+      <c r="B41" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="57"/>
-      <c r="D41" s="57">
+      <c r="C41" s="40"/>
+      <c r="D41" s="40">
         <v>6</v>
       </c>
-      <c r="E41" s="57" t="s">
+      <c r="E41" s="40" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A42" s="56">
+      <c r="A42" s="39">
         <v>39</v>
       </c>
-      <c r="B42" s="57" t="s">
+      <c r="B42" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="57"/>
-      <c r="D42" s="57">
+      <c r="C42" s="40"/>
+      <c r="D42" s="40">
         <v>6</v>
       </c>
-      <c r="E42" s="57" t="s">
+      <c r="E42" s="40" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A43" s="56">
+      <c r="A43" s="39">
         <v>40</v>
       </c>
-      <c r="B43" s="57" t="s">
+      <c r="B43" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="57"/>
-      <c r="D43" s="57">
+      <c r="C43" s="40"/>
+      <c r="D43" s="40">
         <v>10</v>
       </c>
-      <c r="E43" s="57" t="s">
+      <c r="E43" s="40" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A44" s="56">
+      <c r="A44" s="39">
         <v>41</v>
       </c>
-      <c r="B44" s="57" t="s">
+      <c r="B44" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="57"/>
-      <c r="D44" s="57">
+      <c r="C44" s="40"/>
+      <c r="D44" s="40">
         <v>2</v>
       </c>
-      <c r="E44" s="57" t="s">
+      <c r="E44" s="40" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A45" s="56">
+      <c r="A45" s="39">
         <v>42</v>
       </c>
-      <c r="B45" s="57" t="s">
+      <c r="B45" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="57"/>
-      <c r="D45" s="57">
+      <c r="C45" s="40"/>
+      <c r="D45" s="40">
         <v>5</v>
       </c>
-      <c r="E45" s="57" t="s">
+      <c r="E45" s="40" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A46" s="56">
+      <c r="A46" s="39">
         <v>43</v>
       </c>
-      <c r="B46" s="57" t="s">
+      <c r="B46" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C46" s="57"/>
-      <c r="D46" s="57">
+      <c r="C46" s="40"/>
+      <c r="D46" s="40">
         <v>4</v>
       </c>
-      <c r="E46" s="57" t="s">
+      <c r="E46" s="40" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A47" s="56">
+      <c r="A47" s="39">
         <v>44</v>
       </c>
-      <c r="B47" s="57" t="s">
+      <c r="B47" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C47" s="57"/>
-      <c r="D47" s="57">
+      <c r="C47" s="40"/>
+      <c r="D47" s="40">
         <v>3</v>
       </c>
-      <c r="E47" s="57" t="s">
+      <c r="E47" s="40" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A48" s="56">
+      <c r="A48" s="39">
         <v>45</v>
       </c>
-      <c r="B48" s="57" t="s">
+      <c r="B48" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C48" s="57"/>
-      <c r="D48" s="57">
+      <c r="C48" s="40"/>
+      <c r="D48" s="40">
         <v>6</v>
       </c>
-      <c r="E48" s="57" t="s">
+      <c r="E48" s="40" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A49" s="56">
+      <c r="A49" s="39">
         <v>46</v>
       </c>
-      <c r="B49" s="57" t="s">
+      <c r="B49" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C49" s="57"/>
-      <c r="D49" s="57">
+      <c r="C49" s="40"/>
+      <c r="D49" s="40">
         <v>3</v>
       </c>
-      <c r="E49" s="57" t="s">
+      <c r="E49" s="40" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A50" s="56">
+      <c r="A50" s="39">
         <v>47</v>
       </c>
-      <c r="B50" s="57" t="s">
+      <c r="B50" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="C50" s="57"/>
-      <c r="D50" s="57">
+      <c r="C50" s="40"/>
+      <c r="D50" s="40">
         <v>3</v>
       </c>
-      <c r="E50" s="57" t="s">
+      <c r="E50" s="40" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A51" s="56">
+      <c r="A51" s="39">
         <v>48</v>
       </c>
       <c r="B51" s="32" t="s">
@@ -2051,7 +2051,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A52" s="56">
+      <c r="A52" s="39">
         <v>49</v>
       </c>
       <c r="B52" s="32" t="s">
@@ -2065,69 +2065,69 @@
       <c r="E52" s="29"/>
     </row>
     <row r="53" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A53" s="56">
+      <c r="A53" s="39">
         <v>50</v>
       </c>
-      <c r="B53" s="57" t="s">
+      <c r="B53" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="C53" s="57"/>
-      <c r="D53" s="57"/>
-      <c r="E53" s="57" t="s">
+      <c r="C53" s="40"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="40" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A54" s="56">
+      <c r="A54" s="39">
         <v>51</v>
       </c>
-      <c r="B54" s="57" t="s">
+      <c r="B54" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="C54" s="57"/>
-      <c r="D54" s="57"/>
-      <c r="E54" s="57"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
     </row>
     <row r="55" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A55" s="56">
+      <c r="A55" s="39">
         <v>52</v>
       </c>
-      <c r="B55" s="57" t="s">
+      <c r="B55" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C55" s="57"/>
-      <c r="D55" s="57">
+      <c r="C55" s="40"/>
+      <c r="D55" s="40">
         <v>10</v>
       </c>
-      <c r="E55" s="57"/>
+      <c r="E55" s="40"/>
     </row>
     <row r="56" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A56" s="56">
+      <c r="A56" s="39">
         <v>53</v>
       </c>
-      <c r="B56" s="57" t="s">
+      <c r="B56" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="57"/>
-      <c r="D56" s="57">
+      <c r="C56" s="40"/>
+      <c r="D56" s="40">
         <v>48</v>
       </c>
-      <c r="E56" s="57" t="s">
+      <c r="E56" s="40" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A57" s="56">
+      <c r="A57" s="39">
         <v>54</v>
       </c>
-      <c r="B57" s="57" t="s">
+      <c r="B57" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C57" s="57"/>
-      <c r="D57" s="57">
+      <c r="C57" s="40"/>
+      <c r="D57" s="40">
         <v>3</v>
       </c>
-      <c r="E57" s="57" t="s">
+      <c r="E57" s="40" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2152,7 +2152,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:A36"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2167,15 +2167,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="41"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:7" ht="30.75" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -2355,17 +2355,17 @@
       <c r="A11" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="44"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="57"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="49" t="s">
         <v>87</v>
       </c>
       <c r="B12" s="3">
@@ -2386,7 +2386,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A13" s="46"/>
+      <c r="A13" s="58"/>
       <c r="B13" s="3">
         <v>8</v>
       </c>
@@ -2405,7 +2405,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A14" s="46"/>
+      <c r="A14" s="58"/>
       <c r="B14" s="3">
         <v>9</v>
       </c>
@@ -2424,7 +2424,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A15" s="46"/>
+      <c r="A15" s="58"/>
       <c r="B15" s="3">
         <v>10</v>
       </c>
@@ -2443,7 +2443,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A16" s="46"/>
+      <c r="A16" s="58"/>
       <c r="B16" s="3">
         <v>11</v>
       </c>
@@ -2462,7 +2462,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="30.75" thickBot="1">
-      <c r="A17" s="46"/>
+      <c r="A17" s="58"/>
       <c r="B17" s="9">
         <v>12</v>
       </c>
@@ -2481,7 +2481,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A18" s="46"/>
+      <c r="A18" s="58"/>
       <c r="B18" s="9">
         <v>13</v>
       </c>
@@ -2500,7 +2500,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="30.75" thickBot="1">
-      <c r="A19" s="46"/>
+      <c r="A19" s="58"/>
       <c r="B19" s="9">
         <v>14</v>
       </c>
@@ -2519,7 +2519,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="30">
-      <c r="A20" s="46"/>
+      <c r="A20" s="58"/>
       <c r="B20" s="18">
         <v>15</v>
       </c>
@@ -2538,7 +2538,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="30">
-      <c r="A21" s="46"/>
+      <c r="A21" s="58"/>
       <c r="B21" s="19"/>
       <c r="C21" s="34" t="s">
         <v>118</v>
@@ -2555,7 +2555,7 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="46"/>
+      <c r="A22" s="58"/>
       <c r="B22" s="30">
         <v>16</v>
       </c>
@@ -2574,7 +2574,7 @@
       <c r="I22" s="21"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="47"/>
+      <c r="A23" s="59"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
       <c r="D23" s="20">
@@ -2589,105 +2589,111 @@
       <c r="A24" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="48" t="s">
+      <c r="B24" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="49"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="51"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="63"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="B25" s="56">
+      <c r="B25" s="39">
         <v>17</v>
       </c>
-      <c r="C25" s="57" t="s">
+      <c r="C25" s="40" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="28">
         <v>10</v>
       </c>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58" t="s">
+      <c r="E25" s="41"/>
+      <c r="F25" s="41" t="s">
         <v>134</v>
       </c>
       <c r="G25" s="30"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A26" s="64"/>
-      <c r="B26" s="56">
+      <c r="A26" s="50"/>
+      <c r="B26" s="39">
         <v>18</v>
       </c>
-      <c r="C26" s="57" t="s">
+      <c r="C26" s="40" t="s">
         <v>120</v>
       </c>
       <c r="D26" s="3">
         <v>3</v>
       </c>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58" t="s">
+      <c r="E26" s="41"/>
+      <c r="F26" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="G26" s="30"/>
+      <c r="G26" s="30" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A27" s="64"/>
-      <c r="B27" s="56">
+      <c r="A27" s="50"/>
+      <c r="B27" s="39">
         <v>19</v>
       </c>
-      <c r="C27" s="57" t="s">
+      <c r="C27" s="40" t="s">
         <v>80</v>
       </c>
       <c r="D27" s="3">
         <v>10</v>
       </c>
-      <c r="E27" s="58"/>
-      <c r="F27" s="58" t="s">
+      <c r="E27" s="41"/>
+      <c r="F27" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="G27" s="30"/>
+      <c r="G27" s="30" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A28" s="64"/>
-      <c r="B28" s="56">
+      <c r="A28" s="50"/>
+      <c r="B28" s="39">
         <v>20</v>
       </c>
-      <c r="C28" s="57" t="s">
+      <c r="C28" s="40" t="s">
         <v>136</v>
       </c>
       <c r="D28" s="3">
         <v>13</v>
       </c>
-      <c r="E28" s="58"/>
-      <c r="F28" s="58" t="s">
+      <c r="E28" s="41"/>
+      <c r="F28" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="G28" s="30"/>
+      <c r="G28" s="30" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="30">
-      <c r="A29" s="64"/>
+      <c r="A29" s="50"/>
       <c r="B29" s="31">
         <v>15</v>
       </c>
-      <c r="C29" s="60" t="s">
+      <c r="C29" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="60">
+      <c r="D29" s="43">
         <v>2</v>
       </c>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60" t="s">
+      <c r="E29" s="43"/>
+      <c r="F29" s="43" t="s">
         <v>67</v>
       </c>
       <c r="G29" s="30"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A30" s="64"/>
-      <c r="B30" s="56">
+      <c r="A30" s="50"/>
+      <c r="B30" s="39">
         <v>21</v>
       </c>
       <c r="C30" s="36" t="s">
@@ -2696,15 +2702,15 @@
       <c r="D30" s="36">
         <v>13</v>
       </c>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57" t="s">
+      <c r="E30" s="40"/>
+      <c r="F30" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="G30" s="57"/>
+      <c r="G30" s="40"/>
     </row>
     <row r="31" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A31" s="64"/>
-      <c r="B31" s="56">
+      <c r="A31" s="50"/>
+      <c r="B31" s="39">
         <v>22</v>
       </c>
       <c r="C31" s="36" t="s">
@@ -2713,15 +2719,15 @@
       <c r="D31" s="36">
         <v>8</v>
       </c>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57" t="s">
+      <c r="E31" s="40"/>
+      <c r="F31" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="G31" s="57"/>
+      <c r="G31" s="40"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A32" s="64"/>
-      <c r="B32" s="56">
+      <c r="A32" s="50"/>
+      <c r="B32" s="39">
         <v>23</v>
       </c>
       <c r="C32" s="36" t="s">
@@ -2730,15 +2736,15 @@
       <c r="D32" s="36">
         <v>8</v>
       </c>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57" t="s">
+      <c r="E32" s="40"/>
+      <c r="F32" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="G32" s="57"/>
+      <c r="G32" s="40"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A33" s="64"/>
-      <c r="B33" s="56">
+      <c r="A33" s="50"/>
+      <c r="B33" s="39">
         <v>24</v>
       </c>
       <c r="C33" s="36" t="s">
@@ -2747,15 +2753,15 @@
       <c r="D33" s="36">
         <v>8</v>
       </c>
-      <c r="E33" s="57"/>
-      <c r="F33" s="57" t="s">
+      <c r="E33" s="40"/>
+      <c r="F33" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="G33" s="57"/>
+      <c r="G33" s="40"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A34" s="64"/>
-      <c r="B34" s="56">
+      <c r="A34" s="50"/>
+      <c r="B34" s="39">
         <v>28</v>
       </c>
       <c r="C34" s="36" t="s">
@@ -2764,41 +2770,41 @@
       <c r="D34" s="36">
         <v>13</v>
       </c>
-      <c r="E34" s="57"/>
-      <c r="F34" s="57" t="s">
+      <c r="E34" s="40"/>
+      <c r="F34" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="G34" s="57"/>
+      <c r="G34" s="40"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A35" s="64"/>
+      <c r="A35" s="50"/>
       <c r="D35">
         <f>SUM(D25:D34)</f>
         <v>88</v>
       </c>
-      <c r="G35" s="57"/>
+      <c r="G35" s="40"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A36" s="65"/>
-      <c r="B36" s="61"/>
-      <c r="C36" s="62"/>
-      <c r="D36" s="62"/>
-      <c r="E36" s="62"/>
-      <c r="F36" s="62"/>
-      <c r="G36" s="63"/>
+      <c r="A36" s="51"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="54"/>
     </row>
     <row r="37" spans="1:7" ht="29.25" thickBot="1">
       <c r="A37" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="54" t="s">
+      <c r="B37" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="C37" s="55"/>
-      <c r="D37" s="55"/>
-      <c r="E37" s="55"/>
-      <c r="F37" s="55"/>
-      <c r="G37" s="55"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2832,12 +2838,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24" thickBot="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
     </row>
     <row r="2" spans="1:4" ht="20.25" thickBot="1">
       <c r="A2" s="12" t="s">
@@ -2885,13 +2891,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="41"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="46"/>
     </row>
     <row r="2" spans="1:5" ht="30">
       <c r="A2" s="22" t="s">

</xml_diff>

<commit_message>
scrum actualizado 1 julio
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="137">
   <si>
     <t>Product Backlog Items-Prototipo de Realidad Aumentada</t>
   </si>
@@ -278,9 +278,6 @@
     <t>23/12/13 - 03/02/14</t>
   </si>
   <si>
-    <t>Sprint 07/02/14 - 18/03/14</t>
-  </si>
-  <si>
     <t>Realizar relevamiento de informacion. En total 27 dias en este sprint.</t>
   </si>
   <si>
@@ -416,16 +413,22 @@
     <t xml:space="preserve">Configuracion del servidor </t>
   </si>
   <si>
-    <t>Sprint 31/04/14 - 30/05/14</t>
-  </si>
-  <si>
     <t>Investigar conexión del dispositivo android con una base de datos local y realizar la conexión.</t>
   </si>
   <si>
-    <t>Sprint 9/06/14 - 7/07/14</t>
-  </si>
-  <si>
     <t>Agrendizaje de la plataforma .Net</t>
+  </si>
+  <si>
+    <t>Sprint 02  07/02/14 - 18/03/14</t>
+  </si>
+  <si>
+    <t>Sprint 03 31/04/14 - 30/05/14</t>
+  </si>
+  <si>
+    <t>Sprint 04 9/06/14 - 1/07/14</t>
+  </si>
+  <si>
+    <t>Sprint 05 2/07/14 - 31/07/14</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -571,6 +574,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -805,7 +820,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -890,9 +905,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -900,12 +912,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -943,6 +949,9 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -952,26 +961,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1005,8 +1014,30 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1014,6 +1045,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCFF"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1304,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:D37"/>
+    <sheetView topLeftCell="A29" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1318,13 +1354,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="53"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5" ht="30.75" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -1355,96 +1391,96 @@
         <v>72</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A4" s="42">
+      <c r="A4" s="39">
         <v>1</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43">
+      <c r="C4" s="40"/>
+      <c r="D4" s="40">
         <v>10</v>
       </c>
-      <c r="E4" s="43" t="s">
-        <v>90</v>
+      <c r="E4" s="40" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A5" s="42">
+      <c r="A5" s="39">
         <v>2</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43">
+      <c r="C5" s="40"/>
+      <c r="D5" s="40">
         <v>2</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="40" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A6" s="42">
+      <c r="A6" s="39">
         <v>3</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43">
+      <c r="C6" s="40"/>
+      <c r="D6" s="40">
         <v>5</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="40" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A7" s="42">
+      <c r="A7" s="39">
         <v>4</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43">
+      <c r="C7" s="40"/>
+      <c r="D7" s="40">
         <v>21</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="40" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A8" s="42">
+      <c r="A8" s="39">
         <v>5</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43">
+      <c r="C8" s="40"/>
+      <c r="D8" s="40">
         <v>12</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="40" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A9" s="42">
+      <c r="A9" s="39">
         <v>6</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43">
+      <c r="C9" s="40"/>
+      <c r="D9" s="40">
         <v>16</v>
       </c>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="40" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1475,7 +1511,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45.75" thickBot="1">
@@ -1588,14 +1624,14 @@
         <v>16</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C19" s="26"/>
       <c r="D19" s="26">
         <v>5</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1">
@@ -1606,474 +1642,474 @@
       <c r="E20" s="26"/>
     </row>
     <row r="21" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A21" s="46">
+      <c r="A21" s="43">
         <v>17</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47">
+      <c r="C21" s="44"/>
+      <c r="D21" s="44">
         <v>10</v>
       </c>
-      <c r="E21" s="47" t="s">
-        <v>133</v>
+      <c r="E21" s="44" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A22" s="46">
+      <c r="A22" s="43">
         <v>18</v>
       </c>
-      <c r="B22" s="48" t="s">
-        <v>117</v>
-      </c>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47">
+      <c r="B22" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44">
         <v>3</v>
       </c>
-      <c r="E22" s="47" t="s">
+      <c r="E22" s="44" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A23" s="46">
+      <c r="A23" s="43">
         <v>19</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47">
+      <c r="C23" s="44"/>
+      <c r="D23" s="44">
         <v>10</v>
       </c>
-      <c r="E23" s="47"/>
+      <c r="E23" s="44"/>
     </row>
     <row r="24" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A24" s="46">
+      <c r="A24" s="43">
         <v>20</v>
       </c>
-      <c r="B24" s="47" t="s">
-        <v>131</v>
-      </c>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47">
+      <c r="B24" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44">
         <v>13</v>
       </c>
-      <c r="E24" s="47" t="s">
+      <c r="E24" s="44" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A25" s="46">
+      <c r="A25" s="43">
         <v>21</v>
       </c>
-      <c r="B25" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49">
+      <c r="B25" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46">
         <v>13</v>
       </c>
-      <c r="E25" s="50" t="s">
-        <v>103</v>
+      <c r="E25" s="47" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A26" s="46">
+      <c r="A26" s="43">
         <v>22</v>
       </c>
-      <c r="B26" s="49" t="s">
+      <c r="B26" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46">
+        <v>8</v>
+      </c>
+      <c r="E26" s="47" t="s">
         <v>112</v>
-      </c>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49">
-        <v>8</v>
-      </c>
-      <c r="E26" s="50" t="s">
-        <v>113</v>
       </c>
       <c r="F26" s="28"/>
       <c r="G26" s="28"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A27" s="46">
+      <c r="A27" s="43">
         <v>23</v>
       </c>
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46">
+        <v>7</v>
+      </c>
+      <c r="E27" s="47" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A28" s="43">
+        <v>24</v>
+      </c>
+      <c r="B28" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49">
+      <c r="C28" s="46"/>
+      <c r="D28" s="46">
+        <v>8</v>
+      </c>
+      <c r="E28" s="47" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A29" s="73">
+        <v>25</v>
+      </c>
+      <c r="B29" s="71" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" s="71"/>
+      <c r="D29" s="71">
+        <v>11</v>
+      </c>
+      <c r="E29" s="72" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A30" s="73">
+        <v>26</v>
+      </c>
+      <c r="B30" s="71" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71">
+        <v>15</v>
+      </c>
+      <c r="E30" s="72" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A31" s="43">
+        <v>28</v>
+      </c>
+      <c r="B31" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46">
+        <v>13</v>
+      </c>
+      <c r="E31" s="47" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A32" s="75">
+        <v>29</v>
+      </c>
+      <c r="B32" s="79" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" s="80"/>
+      <c r="D32" s="80">
+        <v>2</v>
+      </c>
+      <c r="E32" s="81" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A33" s="35">
+        <v>30</v>
+      </c>
+      <c r="B33" s="71" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71">
+        <v>8</v>
+      </c>
+      <c r="E33" s="72" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="45.75" thickBot="1">
+      <c r="A34" s="73">
+        <v>31</v>
+      </c>
+      <c r="B34" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="72"/>
+      <c r="D34" s="71">
+        <v>13</v>
+      </c>
+      <c r="E34" s="72" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30.75" thickBot="1">
+      <c r="A35" s="75">
+        <v>32</v>
+      </c>
+      <c r="B35" s="77" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="77"/>
+      <c r="D35" s="77">
+        <v>10</v>
+      </c>
+      <c r="E35" s="78" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30.75" thickBot="1">
+      <c r="A36" s="73">
+        <v>33</v>
+      </c>
+      <c r="B36" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="71"/>
+      <c r="D36" s="71">
         <v>7</v>
       </c>
-      <c r="E27" s="50" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A28" s="46">
+      <c r="E36" s="72" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A37" s="73">
+        <v>34</v>
+      </c>
+      <c r="B37" s="71" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" s="71"/>
+      <c r="D37" s="71">
+        <v>9</v>
+      </c>
+      <c r="E37" s="72"/>
+    </row>
+    <row r="38" spans="1:5" ht="30.75" thickBot="1">
+      <c r="A38" s="73">
+        <v>35</v>
+      </c>
+      <c r="B38" s="71" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="71"/>
+      <c r="D38" s="71">
+        <v>4</v>
+      </c>
+      <c r="E38" s="72" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30.75" thickBot="1">
+      <c r="A39" s="73">
+        <v>36</v>
+      </c>
+      <c r="B39" s="71" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39" s="71"/>
+      <c r="D39" s="71">
+        <v>6</v>
+      </c>
+      <c r="E39" s="72" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30.75" thickBot="1">
+      <c r="A40" s="75">
+        <v>37</v>
+      </c>
+      <c r="B40" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="76"/>
+      <c r="D40" s="76">
+        <v>7</v>
+      </c>
+      <c r="E40" s="76" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="30.75" thickBot="1">
+      <c r="A41" s="75">
+        <v>38</v>
+      </c>
+      <c r="B41" s="76" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="76"/>
+      <c r="D41" s="76">
+        <v>6</v>
+      </c>
+      <c r="E41" s="76" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A42" s="75">
+        <v>39</v>
+      </c>
+      <c r="B42" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="76"/>
+      <c r="D42" s="76">
+        <v>6</v>
+      </c>
+      <c r="E42" s="76" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30.75" thickBot="1">
+      <c r="A43" s="75">
+        <v>40</v>
+      </c>
+      <c r="B43" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="76"/>
+      <c r="D43" s="76">
+        <v>10</v>
+      </c>
+      <c r="E43" s="76" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30.75" thickBot="1">
+      <c r="A44" s="35">
+        <v>41</v>
+      </c>
+      <c r="B44" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36">
+        <v>2</v>
+      </c>
+      <c r="E44" s="36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A45" s="75">
+        <v>42</v>
+      </c>
+      <c r="B45" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="76"/>
+      <c r="D45" s="76">
+        <v>5</v>
+      </c>
+      <c r="E45" s="76" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A46" s="35">
+        <v>43</v>
+      </c>
+      <c r="B46" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49">
-        <v>8</v>
-      </c>
-      <c r="E28" s="50" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A29" s="38">
+      <c r="C46" s="36"/>
+      <c r="D46" s="36">
+        <v>4</v>
+      </c>
+      <c r="E46" s="36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A47" s="35">
+        <v>44</v>
+      </c>
+      <c r="B47" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35">
-        <v>11</v>
-      </c>
-      <c r="E29" s="36" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A30" s="38">
+      <c r="C47" s="36"/>
+      <c r="D47" s="36">
+        <v>3</v>
+      </c>
+      <c r="E47" s="36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A48" s="35">
+        <v>45</v>
+      </c>
+      <c r="B48" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35">
-        <v>15</v>
-      </c>
-      <c r="E30" s="36" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A31" s="46">
-        <v>28</v>
-      </c>
-      <c r="B31" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49">
+      <c r="C48" s="36"/>
+      <c r="D48" s="36">
+        <v>6</v>
+      </c>
+      <c r="E48" s="36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A49" s="35">
+        <v>46</v>
+      </c>
+      <c r="B49" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36">
+        <v>3</v>
+      </c>
+      <c r="E49" s="36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="30.75" thickBot="1">
+      <c r="A50" s="41">
+        <v>47</v>
+      </c>
+      <c r="B50" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" s="42"/>
+      <c r="D50" s="42">
+        <v>3</v>
+      </c>
+      <c r="E50" s="42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A51" s="75">
+        <v>48</v>
+      </c>
+      <c r="B51" s="79" t="s">
+        <v>126</v>
+      </c>
+      <c r="C51" s="80"/>
+      <c r="D51" s="80">
         <v>13</v>
       </c>
-      <c r="E31" s="50" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A32" s="38">
-        <v>29</v>
-      </c>
-      <c r="B32" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28">
-        <v>2</v>
-      </c>
-      <c r="E32" s="32" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A33" s="38">
-        <v>30</v>
-      </c>
-      <c r="B33" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" s="35"/>
-      <c r="D33" s="35">
-        <v>8</v>
-      </c>
-      <c r="E33" s="36" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A34" s="38">
-        <v>31</v>
-      </c>
-      <c r="B34" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="35">
-        <v>13</v>
-      </c>
-      <c r="E34" s="36" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A35" s="38">
-        <v>32</v>
-      </c>
-      <c r="B35" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="C35" s="35"/>
-      <c r="D35" s="35">
-        <v>10</v>
-      </c>
-      <c r="E35" s="36" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A36" s="38">
-        <v>33</v>
-      </c>
-      <c r="B36" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35">
-        <v>7</v>
-      </c>
-      <c r="E36" s="36" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A37" s="38">
-        <v>34</v>
-      </c>
-      <c r="B37" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35">
-        <v>9</v>
-      </c>
-      <c r="E37" s="36"/>
-    </row>
-    <row r="38" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A38" s="38">
-        <v>35</v>
-      </c>
-      <c r="B38" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35">
-        <v>4</v>
-      </c>
-      <c r="E38" s="36" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A39" s="38">
-        <v>36</v>
-      </c>
-      <c r="B39" s="35" t="s">
-        <v>121</v>
-      </c>
-      <c r="C39" s="35"/>
-      <c r="D39" s="35">
-        <v>6</v>
-      </c>
-      <c r="E39" s="36" t="s">
+      <c r="E51" s="81" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A52" s="35">
+        <v>49</v>
+      </c>
+      <c r="B52" s="31" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A40" s="38">
-        <v>37</v>
-      </c>
-      <c r="B40" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="C40" s="39"/>
-      <c r="D40" s="39">
-        <v>7</v>
-      </c>
-      <c r="E40" s="39" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A41" s="38">
-        <v>38</v>
-      </c>
-      <c r="B41" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39">
-        <v>6</v>
-      </c>
-      <c r="E41" s="39" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A42" s="38">
-        <v>39</v>
-      </c>
-      <c r="B42" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39">
-        <v>6</v>
-      </c>
-      <c r="E42" s="39" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A43" s="38">
-        <v>40</v>
-      </c>
-      <c r="B43" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39">
-        <v>10</v>
-      </c>
-      <c r="E43" s="39" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A44" s="38">
-        <v>41</v>
-      </c>
-      <c r="B44" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39">
-        <v>2</v>
-      </c>
-      <c r="E44" s="39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A45" s="38">
-        <v>42</v>
-      </c>
-      <c r="B45" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39">
-        <v>5</v>
-      </c>
-      <c r="E45" s="39" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A46" s="38">
-        <v>43</v>
-      </c>
-      <c r="B46" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39">
-        <v>4</v>
-      </c>
-      <c r="E46" s="39" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A47" s="38">
-        <v>44</v>
-      </c>
-      <c r="B47" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C47" s="39"/>
-      <c r="D47" s="39">
-        <v>3</v>
-      </c>
-      <c r="E47" s="39" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A48" s="38">
-        <v>45</v>
-      </c>
-      <c r="B48" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="C48" s="39"/>
-      <c r="D48" s="39">
-        <v>6</v>
-      </c>
-      <c r="E48" s="39" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A49" s="38">
-        <v>46</v>
-      </c>
-      <c r="B49" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C49" s="39"/>
-      <c r="D49" s="39">
-        <v>3</v>
-      </c>
-      <c r="E49" s="39" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A50" s="44">
-        <v>47</v>
-      </c>
-      <c r="B50" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45">
-        <v>3</v>
-      </c>
-      <c r="E50" s="45" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A51" s="38">
-        <v>48</v>
-      </c>
-      <c r="B51" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="C51" s="28"/>
-      <c r="D51" s="28">
-        <v>13</v>
-      </c>
-      <c r="E51" s="32" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A52" s="38">
-        <v>49</v>
-      </c>
-      <c r="B52" s="31" t="s">
-        <v>123</v>
       </c>
       <c r="C52" s="28"/>
       <c r="D52" s="28">
@@ -2083,69 +2119,69 @@
       <c r="E52" s="28"/>
     </row>
     <row r="53" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A53" s="38">
+      <c r="A53" s="35">
         <v>50</v>
       </c>
-      <c r="B53" s="39" t="s">
+      <c r="B53" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="C53" s="39"/>
-      <c r="D53" s="39"/>
-      <c r="E53" s="39" t="s">
+      <c r="C53" s="36"/>
+      <c r="D53" s="36"/>
+      <c r="E53" s="36" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A54" s="38">
+      <c r="A54" s="35">
         <v>51</v>
       </c>
-      <c r="B54" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="C54" s="39"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="39"/>
+      <c r="B54" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" s="36"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="36"/>
     </row>
     <row r="55" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A55" s="38">
+      <c r="A55" s="35">
         <v>52</v>
       </c>
-      <c r="B55" s="39" t="s">
+      <c r="B55" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="C55" s="39"/>
-      <c r="D55" s="39">
+      <c r="C55" s="36"/>
+      <c r="D55" s="36">
         <v>10</v>
       </c>
-      <c r="E55" s="39"/>
+      <c r="E55" s="36"/>
     </row>
     <row r="56" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A56" s="38">
+      <c r="A56" s="35">
         <v>53</v>
       </c>
-      <c r="B56" s="39" t="s">
+      <c r="B56" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="39"/>
-      <c r="D56" s="39">
+      <c r="C56" s="36"/>
+      <c r="D56" s="36">
         <v>48</v>
       </c>
-      <c r="E56" s="39" t="s">
+      <c r="E56" s="36" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A57" s="38">
+      <c r="A57" s="35">
         <v>54</v>
       </c>
-      <c r="B57" s="39" t="s">
+      <c r="B57" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C57" s="39"/>
-      <c r="D57" s="39">
+      <c r="C57" s="36"/>
+      <c r="D57" s="36">
         <v>3</v>
       </c>
-      <c r="E57" s="39" t="s">
+      <c r="E57" s="36" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2167,10 +2203,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51:G51"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2185,15 +2221,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="53"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51"/>
     </row>
     <row r="2" spans="1:7" ht="30.75" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -2373,18 +2409,18 @@
       <c r="A11" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="64"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="62"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A12" s="56" t="s">
-        <v>86</v>
+      <c r="A12" s="52" t="s">
+        <v>133</v>
       </c>
       <c r="B12" s="3">
         <v>7</v>
@@ -2404,7 +2440,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A13" s="65"/>
+      <c r="A13" s="63"/>
       <c r="B13" s="3">
         <v>8</v>
       </c>
@@ -2423,7 +2459,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A14" s="65"/>
+      <c r="A14" s="63"/>
       <c r="B14" s="3">
         <v>9</v>
       </c>
@@ -2442,7 +2478,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A15" s="65"/>
+      <c r="A15" s="63"/>
       <c r="B15" s="3">
         <v>10</v>
       </c>
@@ -2461,7 +2497,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A16" s="65"/>
+      <c r="A16" s="63"/>
       <c r="B16" s="3">
         <v>11</v>
       </c>
@@ -2480,7 +2516,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="30.75" thickBot="1">
-      <c r="A17" s="65"/>
+      <c r="A17" s="63"/>
       <c r="B17" s="9">
         <v>12</v>
       </c>
@@ -2499,7 +2535,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A18" s="65"/>
+      <c r="A18" s="63"/>
       <c r="B18" s="9">
         <v>13</v>
       </c>
@@ -2518,7 +2554,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="30.75" thickBot="1">
-      <c r="A19" s="65"/>
+      <c r="A19" s="63"/>
       <c r="B19" s="9">
         <v>14</v>
       </c>
@@ -2537,7 +2573,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="30">
-      <c r="A20" s="65"/>
+      <c r="A20" s="63"/>
       <c r="B20" s="18">
         <v>15</v>
       </c>
@@ -2552,39 +2588,39 @@
         <v>66</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="30">
-      <c r="A21" s="65"/>
+      <c r="A21" s="63"/>
       <c r="B21" s="19"/>
-      <c r="C21" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="D21" s="33">
+      <c r="C21" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="32">
         <v>2</v>
       </c>
-      <c r="E21" s="34"/>
-      <c r="F21" s="33" t="s">
-        <v>114</v>
+      <c r="E21" s="33"/>
+      <c r="F21" s="32" t="s">
+        <v>113</v>
       </c>
       <c r="G21" s="19" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="65"/>
+      <c r="A22" s="63"/>
       <c r="B22" s="29">
         <v>16</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D22" s="30">
         <v>5</v>
       </c>
       <c r="F22" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G22" s="29" t="s">
         <v>83</v>
@@ -2592,7 +2628,7 @@
       <c r="I22" s="21"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="66"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
       <c r="D23" s="20">
@@ -2607,68 +2643,68 @@
       <c r="A24" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="67" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="68"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="70"/>
+      <c r="B24" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="66"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="68"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A25" s="56" t="s">
-        <v>132</v>
-      </c>
-      <c r="B25" s="38">
+      <c r="A25" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="35">
         <v>17</v>
       </c>
-      <c r="C25" s="39" t="s">
+      <c r="C25" s="36" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="27">
         <v>10</v>
       </c>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40" t="s">
-        <v>129</v>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37" t="s">
+        <v>128</v>
       </c>
       <c r="G25" s="29" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A26" s="57"/>
-      <c r="B26" s="38">
+      <c r="A26" s="53"/>
+      <c r="B26" s="35">
         <v>18</v>
       </c>
-      <c r="C26" s="39" t="s">
-        <v>117</v>
+      <c r="C26" s="36" t="s">
+        <v>116</v>
       </c>
       <c r="D26" s="3">
         <v>3</v>
       </c>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40" t="s">
-        <v>130</v>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37" t="s">
+        <v>129</v>
       </c>
       <c r="G26" s="29" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A27" s="57"/>
-      <c r="B27" s="38">
+      <c r="A27" s="53"/>
+      <c r="B27" s="35">
         <v>19</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C27" s="36" t="s">
         <v>79</v>
       </c>
       <c r="D27" s="3">
         <v>10</v>
       </c>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40" t="s">
+      <c r="E27" s="37"/>
+      <c r="F27" s="37" t="s">
         <v>67</v>
       </c>
       <c r="G27" s="29" t="s">
@@ -2676,37 +2712,37 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A28" s="57"/>
-      <c r="B28" s="38">
+      <c r="A28" s="53"/>
+      <c r="B28" s="35">
         <v>20</v>
       </c>
-      <c r="C28" s="39" t="s">
-        <v>131</v>
+      <c r="C28" s="36" t="s">
+        <v>130</v>
       </c>
       <c r="D28" s="3">
         <v>13</v>
       </c>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40" t="s">
-        <v>114</v>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37" t="s">
+        <v>113</v>
       </c>
       <c r="G28" s="29" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="30">
-      <c r="A29" s="57"/>
+      <c r="A29" s="53"/>
       <c r="B29" s="30">
         <v>15</v>
       </c>
-      <c r="C29" s="41" t="s">
+      <c r="C29" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="41">
+      <c r="D29" s="38">
         <v>2</v>
       </c>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41" t="s">
+      <c r="E29" s="38"/>
+      <c r="F29" s="38" t="s">
         <v>66</v>
       </c>
       <c r="G29" s="29" t="s">
@@ -2714,301 +2750,482 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A30" s="57"/>
-      <c r="B30" s="38">
+      <c r="A30" s="53"/>
+      <c r="B30" s="35">
         <v>21</v>
       </c>
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="34">
+        <v>13</v>
+      </c>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="G30" s="36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A31" s="53"/>
+      <c r="B31" s="35">
+        <v>23</v>
+      </c>
+      <c r="C31" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="35">
+      <c r="D31" s="34">
+        <v>8</v>
+      </c>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="G31" s="36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A32" s="53"/>
+      <c r="B32" s="35">
+        <v>24</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="34">
+        <v>8</v>
+      </c>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" s="36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A33" s="53"/>
+      <c r="B33" s="35">
+        <v>28</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" s="34">
         <v>13</v>
       </c>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="G30" s="39" t="s">
+      <c r="E33" s="36"/>
+      <c r="F33" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="G33" s="36" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A31" s="57"/>
-      <c r="B31" s="38">
-        <v>23</v>
-      </c>
-      <c r="C31" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" s="35">
-        <v>8</v>
-      </c>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="G31" s="39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A32" s="57"/>
-      <c r="B32" s="38">
-        <v>24</v>
-      </c>
-      <c r="C32" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" s="35">
-        <v>8</v>
-      </c>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="G32" s="39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A33" s="57"/>
-      <c r="B33" s="38">
-        <v>28</v>
-      </c>
-      <c r="C33" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="D33" s="35">
-        <v>13</v>
-      </c>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="G33" s="39" t="s">
-        <v>83</v>
-      </c>
-    </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="57"/>
+      <c r="A34" s="53"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="57"/>
+      <c r="A35" s="53"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A36" s="57"/>
+      <c r="A36" s="53"/>
       <c r="D36">
         <f>SUM(D25:D33)</f>
         <v>80</v>
       </c>
-      <c r="G36" s="39"/>
+      <c r="G36" s="36"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A37" s="58"/>
-      <c r="B37" s="59"/>
-      <c r="C37" s="60"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
-      <c r="G37" s="61"/>
+      <c r="A37" s="54"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56"/>
+      <c r="G37" s="57"/>
     </row>
     <row r="38" spans="1:7" ht="29.25" thickBot="1">
       <c r="A38" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B38" s="54" t="s">
-        <v>126</v>
-      </c>
-      <c r="C38" s="55"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="55"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
+      <c r="B38" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" s="59"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="59"/>
+      <c r="F38" s="59"/>
+      <c r="G38" s="59"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A39" s="56" t="s">
-        <v>134</v>
-      </c>
-      <c r="B39" s="38">
+      <c r="A39" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" s="35">
         <v>25</v>
       </c>
-      <c r="C39" s="35" t="s">
+      <c r="C39" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39" s="34">
+        <v>11</v>
+      </c>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="G39" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A40" s="53"/>
+      <c r="B40" s="35">
+        <v>26</v>
+      </c>
+      <c r="C40" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="D39" s="35">
-        <v>11</v>
-      </c>
-      <c r="E39" s="40"/>
-      <c r="F39" s="40" t="s">
+      <c r="D40" s="34">
+        <v>15</v>
+      </c>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="G40" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A41" s="53"/>
+      <c r="B41" s="35">
+        <v>30</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" s="34">
+        <v>8</v>
+      </c>
+      <c r="F41" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="G39" s="29"/>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A40" s="57"/>
-      <c r="B40" s="38">
-        <v>26</v>
-      </c>
-      <c r="C40" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="D40" s="35">
-        <v>15</v>
-      </c>
-      <c r="E40" s="40"/>
-      <c r="F40" s="40" t="s">
+      <c r="G41" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A42" s="53"/>
+      <c r="B42" s="35">
+        <v>31</v>
+      </c>
+      <c r="C42" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" s="34">
+        <v>13</v>
+      </c>
+      <c r="F42" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="G40" s="29"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A41" s="57"/>
-      <c r="B41" s="38">
-        <v>30</v>
-      </c>
-      <c r="C41" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="D41" s="35">
-        <v>8</v>
-      </c>
-      <c r="F41" s="40" t="s">
+      <c r="G42" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A43" s="53"/>
+      <c r="B43" s="35">
+        <v>33</v>
+      </c>
+      <c r="C43" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" s="34">
+        <v>7</v>
+      </c>
+      <c r="F43" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="G41" s="29"/>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A42" s="57"/>
-      <c r="B42" s="38">
-        <v>31</v>
-      </c>
-      <c r="C42" s="73" t="s">
-        <v>111</v>
-      </c>
-      <c r="D42" s="35">
-        <v>13</v>
-      </c>
-      <c r="F42" s="40" t="s">
+      <c r="G43" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A44" s="53"/>
+      <c r="B44" s="35">
+        <v>35</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="34">
+        <v>4</v>
+      </c>
+      <c r="F44" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="G44" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A45" s="53"/>
+      <c r="B45" s="35">
+        <v>36</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="D45" s="34">
+        <v>6</v>
+      </c>
+      <c r="F45" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="G42" s="29"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A43" s="57"/>
-      <c r="B43" s="38">
-        <v>33</v>
-      </c>
-      <c r="C43" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="D43" s="35">
-        <v>7</v>
-      </c>
-      <c r="F43" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="G43" s="39"/>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A44" s="57"/>
-      <c r="B44" s="38">
-        <v>35</v>
-      </c>
-      <c r="C44" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="D44" s="35">
-        <v>4</v>
-      </c>
-      <c r="F44" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="G44" s="39"/>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A45" s="57"/>
-      <c r="B45" s="38">
-        <v>36</v>
-      </c>
-      <c r="C45" s="35" t="s">
-        <v>121</v>
-      </c>
-      <c r="D45" s="35">
-        <v>6</v>
-      </c>
-      <c r="F45" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="G45" s="39"/>
+      <c r="G45" s="29" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A46" s="57"/>
-      <c r="B46" s="38">
+      <c r="A46" s="53"/>
+      <c r="B46" s="35">
         <v>34</v>
       </c>
-      <c r="C46" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="D46" s="35">
+      <c r="C46" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="D46" s="34">
         <v>9</v>
       </c>
-      <c r="E46" s="35"/>
-      <c r="F46" s="39" t="s">
+      <c r="E46" s="34"/>
+      <c r="F46" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="G46" s="39"/>
+      <c r="G46" s="29" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A47" s="57"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="35">
+      <c r="A47" s="53"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="34">
         <f>SUM(D39:D46)</f>
         <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A48" s="57"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="35"/>
+      <c r="A48" s="53"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
     </row>
     <row r="49" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A49" s="57"/>
-      <c r="G49" s="39"/>
+      <c r="A49" s="53"/>
+      <c r="G49" s="36"/>
     </row>
     <row r="50" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A50" s="58"/>
-      <c r="B50" s="59"/>
-      <c r="C50" s="60"/>
-      <c r="D50" s="60"/>
-      <c r="E50" s="60"/>
-      <c r="F50" s="60"/>
-      <c r="G50" s="61"/>
+      <c r="A50" s="54"/>
+      <c r="B50" s="55"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="56"/>
+      <c r="E50" s="56"/>
+      <c r="F50" s="56"/>
+      <c r="G50" s="57"/>
     </row>
     <row r="51" spans="1:7" ht="29.25" thickBot="1">
       <c r="A51" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B51" s="54"/>
-      <c r="C51" s="55"/>
-      <c r="D51" s="55"/>
-      <c r="E51" s="55"/>
-      <c r="F51" s="55"/>
-      <c r="G51" s="55"/>
+      <c r="B51" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="C51" s="59"/>
+      <c r="D51" s="59"/>
+      <c r="E51" s="59"/>
+      <c r="F51" s="59"/>
+      <c r="G51" s="59"/>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A52" s="52" t="s">
+        <v>136</v>
+      </c>
+      <c r="B52" s="35">
+        <v>29</v>
+      </c>
+      <c r="C52" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" s="34">
+        <v>2</v>
+      </c>
+      <c r="E52" s="37"/>
+      <c r="F52" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="G52" s="29"/>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A53" s="53"/>
+      <c r="B53" s="35">
+        <v>32</v>
+      </c>
+      <c r="C53" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" s="34">
+        <v>10</v>
+      </c>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="G53" s="29"/>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A54" s="53"/>
+      <c r="B54" s="35">
+        <v>48</v>
+      </c>
+      <c r="C54" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="D54" s="34">
+        <v>13</v>
+      </c>
+      <c r="F54" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="G54" s="29"/>
+    </row>
+    <row r="55" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A55" s="53"/>
+      <c r="B55" s="35">
+        <v>42</v>
+      </c>
+      <c r="C55" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="34">
+        <v>5</v>
+      </c>
+      <c r="F55" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="G55" s="29"/>
+    </row>
+    <row r="56" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A56" s="53"/>
+      <c r="B56" s="35">
+        <v>37</v>
+      </c>
+      <c r="C56" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="34">
+        <v>7</v>
+      </c>
+      <c r="F56" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="G56" s="29"/>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A57" s="53"/>
+      <c r="B57" s="35">
+        <v>38</v>
+      </c>
+      <c r="C57" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="34">
+        <v>6</v>
+      </c>
+      <c r="F57" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="G57" s="29"/>
+    </row>
+    <row r="58" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A58" s="53"/>
+      <c r="B58" s="35">
+        <v>39</v>
+      </c>
+      <c r="C58" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D58" s="34">
+        <v>6</v>
+      </c>
+      <c r="F58" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="G58" s="29"/>
+    </row>
+    <row r="59" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A59" s="53"/>
+      <c r="B59" s="35">
+        <v>40</v>
+      </c>
+      <c r="C59" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D59" s="34">
+        <v>10</v>
+      </c>
+      <c r="E59" s="34"/>
+      <c r="F59" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="G59" s="29"/>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A60" s="53"/>
+      <c r="B60" s="35"/>
+      <c r="C60" s="34"/>
+      <c r="D60" s="34">
+        <f>SUM(D52:D59)</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A61" s="53"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="34"/>
+    </row>
+    <row r="62" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A62" s="53"/>
+      <c r="G62" s="36"/>
+    </row>
+    <row r="63" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A63" s="54"/>
+      <c r="B63" s="55"/>
+      <c r="C63" s="56"/>
+      <c r="D63" s="56"/>
+      <c r="E63" s="56"/>
+      <c r="F63" s="56"/>
+      <c r="G63" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="A12:A23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="A52:A63"/>
+    <mergeCell ref="B63:G63"/>
     <mergeCell ref="A39:A50"/>
     <mergeCell ref="B50:G50"/>
     <mergeCell ref="B51:G51"/>
     <mergeCell ref="B38:G38"/>
     <mergeCell ref="A25:A37"/>
     <mergeCell ref="B37:G37"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="A12:A23"/>
-    <mergeCell ref="B24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3032,12 +3249,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24" thickBot="1">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
     </row>
     <row r="2" spans="1:4" ht="20.25" thickBot="1">
       <c r="A2" s="12" t="s">
@@ -3085,13 +3302,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="53"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5" ht="30">
       <c r="A2" s="22" t="s">

</xml_diff>

<commit_message>
Eliminacion de ANTEPROYECTO FINAL-Correcciones_Mayo_2014.docx y reubicado en otra carpeta
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="137">
   <si>
     <t>Product Backlog Items-Prototipo de Realidad Aumentada</t>
   </si>
@@ -952,68 +952,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1038,6 +976,68 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1338,31 +1338,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" customWidth="1"/>
     <col min="2" max="2" width="69" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="76.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="76.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="51"/>
-    </row>
-    <row r="2" spans="1:5" ht="30.75" thickBot="1">
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="62"/>
+    </row>
+    <row r="2" spans="1:4" ht="30.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1370,755 +1368,702 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3">
+      <c r="C3" s="3">
         <v>72</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30.75" thickBot="1">
+    <row r="4" spans="1:4" ht="30.75" thickBot="1">
       <c r="A4" s="39">
         <v>1</v>
       </c>
       <c r="B4" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40">
+      <c r="C4" s="40">
         <v>10</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="D4" s="40" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1">
+    <row r="5" spans="1:4" ht="15.75" thickBot="1">
       <c r="A5" s="39">
         <v>2</v>
       </c>
       <c r="B5" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40">
+      <c r="C5" s="40">
         <v>2</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="D5" s="40" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1">
       <c r="A6" s="39">
         <v>3</v>
       </c>
       <c r="B6" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40">
+      <c r="C6" s="40">
         <v>5</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="D6" s="40" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1">
       <c r="A7" s="39">
         <v>4</v>
       </c>
       <c r="B7" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40">
+      <c r="C7" s="40">
         <v>21</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="D7" s="40" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1">
       <c r="A8" s="39">
         <v>5</v>
       </c>
       <c r="B8" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40">
+      <c r="C8" s="40">
         <v>12</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="D8" s="40" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30.75" thickBot="1">
+    <row r="9" spans="1:4" ht="30.75" thickBot="1">
       <c r="A9" s="39">
         <v>6</v>
       </c>
       <c r="B9" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40">
+      <c r="C9" s="40">
         <v>16</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="D9" s="40" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1">
       <c r="A10" s="25">
         <v>7</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26">
+      <c r="C10" s="26">
         <v>4</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="D10" s="26" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1">
       <c r="A11" s="25">
         <v>8</v>
       </c>
       <c r="B11" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26">
+      <c r="C11" s="26">
         <v>5</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="D11" s="26" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="45.75" thickBot="1">
+    <row r="12" spans="1:4" ht="45.75" thickBot="1">
       <c r="A12" s="25">
         <v>9</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26">
+      <c r="C12" s="26">
         <v>14</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="D12" s="26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30.75" thickBot="1">
+    <row r="13" spans="1:4" ht="30.75" thickBot="1">
       <c r="A13" s="25">
         <v>10</v>
       </c>
       <c r="B13" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26">
+      <c r="C13" s="26">
         <v>6</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="D13" s="26" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1">
+    <row r="14" spans="1:4" ht="15.75" thickBot="1">
       <c r="A14" s="25">
         <v>11</v>
       </c>
       <c r="B14" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26">
+      <c r="C14" s="26">
         <v>6</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="D14" s="26" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1">
+    <row r="15" spans="1:4" ht="15.75" thickBot="1">
       <c r="A15" s="25">
         <v>12</v>
       </c>
       <c r="B15" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26">
+      <c r="C15" s="26">
         <v>3</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="D15" s="26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1">
+    <row r="16" spans="1:4" ht="15.75" thickBot="1">
       <c r="A16" s="25">
         <v>13</v>
       </c>
       <c r="B16" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26">
+      <c r="C16" s="26">
         <v>10</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="D16" s="26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30.75" thickBot="1">
+    <row r="17" spans="1:6" ht="30.75" thickBot="1">
       <c r="A17" s="25">
         <v>14</v>
       </c>
       <c r="B17" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26">
+      <c r="C17" s="26">
         <v>4</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="D17" s="26" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30.75" thickBot="1">
+    <row r="18" spans="1:6" ht="30.75" thickBot="1">
       <c r="A18" s="25">
         <v>15</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26">
+      <c r="C18" s="26">
         <v>2</v>
       </c>
-      <c r="E18" s="26" t="s">
+      <c r="D18" s="26" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1">
+    <row r="19" spans="1:6" ht="15.75" thickBot="1">
       <c r="A19" s="25">
         <v>16</v>
       </c>
       <c r="B19" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26">
+      <c r="C19" s="26">
         <v>5</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="D19" s="26" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1">
+    <row r="20" spans="1:6" ht="15.75" thickBot="1">
       <c r="A20" s="25"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-    </row>
-    <row r="21" spans="1:7" ht="30.75" thickBot="1">
+    </row>
+    <row r="21" spans="1:6" ht="30.75" thickBot="1">
       <c r="A21" s="43">
         <v>17</v>
       </c>
       <c r="B21" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44">
+      <c r="C21" s="44">
         <v>10</v>
       </c>
-      <c r="E21" s="44" t="s">
+      <c r="D21" s="44" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1">
+    <row r="22" spans="1:6" ht="15.75" thickBot="1">
       <c r="A22" s="43">
         <v>18</v>
       </c>
       <c r="B22" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44">
+      <c r="C22" s="44">
         <v>3</v>
       </c>
-      <c r="E22" s="44" t="s">
+      <c r="D22" s="44" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1">
+    <row r="23" spans="1:6" ht="15.75" thickBot="1">
       <c r="A23" s="43">
         <v>19</v>
       </c>
       <c r="B23" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44">
+      <c r="C23" s="44">
         <v>10</v>
       </c>
-      <c r="E23" s="44"/>
-    </row>
-    <row r="24" spans="1:7" ht="30.75" thickBot="1">
+      <c r="D23" s="44"/>
+    </row>
+    <row r="24" spans="1:6" ht="30.75" thickBot="1">
       <c r="A24" s="43">
         <v>20</v>
       </c>
       <c r="B24" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44">
+      <c r="C24" s="44">
         <v>13</v>
       </c>
-      <c r="E24" s="44" t="s">
+      <c r="D24" s="44" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30.75" thickBot="1">
+    <row r="25" spans="1:6" ht="30.75" thickBot="1">
       <c r="A25" s="43">
         <v>21</v>
       </c>
       <c r="B25" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46">
+      <c r="C25" s="46">
         <v>13</v>
       </c>
-      <c r="E25" s="47" t="s">
+      <c r="D25" s="47" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1">
+    <row r="26" spans="1:6" ht="15.75" thickBot="1">
       <c r="A26" s="43">
         <v>22</v>
       </c>
       <c r="B26" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46">
+      <c r="C26" s="46">
         <v>8</v>
       </c>
-      <c r="E26" s="47" t="s">
+      <c r="D26" s="47" t="s">
         <v>112</v>
       </c>
+      <c r="E26" s="28"/>
       <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1">
+    </row>
+    <row r="27" spans="1:6" ht="15.75" thickBot="1">
       <c r="A27" s="43">
         <v>23</v>
       </c>
       <c r="B27" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46">
+      <c r="C27" s="46">
         <v>7</v>
       </c>
-      <c r="E27" s="47" t="s">
+      <c r="D27" s="47" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1">
+    <row r="28" spans="1:6" ht="15.75" thickBot="1">
       <c r="A28" s="43">
         <v>24</v>
       </c>
       <c r="B28" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46">
+      <c r="C28" s="46">
         <v>8</v>
       </c>
-      <c r="E28" s="47" t="s">
+      <c r="D28" s="47" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A29" s="73">
+    <row r="29" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A29" s="51">
         <v>25</v>
       </c>
-      <c r="B29" s="71" t="s">
+      <c r="B29" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="71"/>
-      <c r="D29" s="71">
+      <c r="C29" s="49">
         <v>11</v>
       </c>
-      <c r="E29" s="72" t="s">
+      <c r="D29" s="50" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A30" s="73">
+    <row r="30" spans="1:6" ht="30.75" thickBot="1">
+      <c r="A30" s="51">
         <v>26</v>
       </c>
-      <c r="B30" s="71" t="s">
+      <c r="B30" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="71"/>
-      <c r="D30" s="71">
+      <c r="C30" s="49">
         <v>15</v>
       </c>
-      <c r="E30" s="72" t="s">
+      <c r="D30" s="50" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30.75" thickBot="1">
+    <row r="31" spans="1:6" ht="30.75" thickBot="1">
       <c r="A31" s="43">
         <v>28</v>
       </c>
       <c r="B31" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46">
+      <c r="C31" s="46">
         <v>13</v>
       </c>
-      <c r="E31" s="47" t="s">
+      <c r="D31" s="47" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A32" s="75">
+    <row r="32" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A32" s="53">
         <v>29</v>
       </c>
-      <c r="B32" s="79" t="s">
+      <c r="B32" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="C32" s="80"/>
-      <c r="D32" s="80">
+      <c r="C32" s="58">
         <v>2</v>
       </c>
-      <c r="E32" s="81" t="s">
+      <c r="D32" s="59" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1">
+    <row r="33" spans="1:4" ht="15.75" thickBot="1">
       <c r="A33" s="35">
         <v>30</v>
       </c>
-      <c r="B33" s="71" t="s">
+      <c r="B33" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="71"/>
-      <c r="D33" s="71">
+      <c r="C33" s="49">
         <v>8</v>
       </c>
-      <c r="E33" s="72" t="s">
+      <c r="D33" s="50" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A34" s="73">
+    <row r="34" spans="1:4" ht="45.75" thickBot="1">
+      <c r="A34" s="51">
         <v>31</v>
       </c>
-      <c r="B34" s="74" t="s">
+      <c r="B34" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="C34" s="72"/>
-      <c r="D34" s="71">
+      <c r="C34" s="49">
         <v>13</v>
       </c>
-      <c r="E34" s="72" t="s">
+      <c r="D34" s="50" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A35" s="75">
+    <row r="35" spans="1:4" ht="30.75" thickBot="1">
+      <c r="A35" s="53">
         <v>32</v>
       </c>
-      <c r="B35" s="77" t="s">
+      <c r="B35" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="77"/>
-      <c r="D35" s="77">
+      <c r="C35" s="55">
         <v>10</v>
       </c>
-      <c r="E35" s="78" t="s">
+      <c r="D35" s="56" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A36" s="73">
+    <row r="36" spans="1:4" ht="30.75" thickBot="1">
+      <c r="A36" s="51">
         <v>33</v>
       </c>
-      <c r="B36" s="71" t="s">
+      <c r="B36" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="C36" s="71"/>
-      <c r="D36" s="71">
+      <c r="C36" s="49">
         <v>7</v>
       </c>
-      <c r="E36" s="72" t="s">
+      <c r="D36" s="50" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A37" s="73">
+    <row r="37" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A37" s="51">
         <v>34</v>
       </c>
-      <c r="B37" s="71" t="s">
+      <c r="B37" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="C37" s="71"/>
-      <c r="D37" s="71">
+      <c r="C37" s="49">
         <v>9</v>
       </c>
-      <c r="E37" s="72"/>
-    </row>
-    <row r="38" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A38" s="73">
+      <c r="D37" s="50"/>
+    </row>
+    <row r="38" spans="1:4" ht="30.75" thickBot="1">
+      <c r="A38" s="51">
         <v>35</v>
       </c>
-      <c r="B38" s="71" t="s">
+      <c r="B38" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="71"/>
-      <c r="D38" s="71">
+      <c r="C38" s="49">
         <v>4</v>
       </c>
-      <c r="E38" s="72" t="s">
+      <c r="D38" s="50" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A39" s="73">
+    <row r="39" spans="1:4" ht="30.75" thickBot="1">
+      <c r="A39" s="51">
         <v>36</v>
       </c>
-      <c r="B39" s="71" t="s">
+      <c r="B39" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="C39" s="71"/>
-      <c r="D39" s="71">
+      <c r="C39" s="49">
         <v>6</v>
       </c>
-      <c r="E39" s="72" t="s">
+      <c r="D39" s="50" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A40" s="75">
+    <row r="40" spans="1:4" ht="30.75" thickBot="1">
+      <c r="A40" s="53">
         <v>37</v>
       </c>
-      <c r="B40" s="76" t="s">
+      <c r="B40" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="76"/>
-      <c r="D40" s="76">
+      <c r="C40" s="54">
         <v>7</v>
       </c>
-      <c r="E40" s="76" t="s">
+      <c r="D40" s="54" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A41" s="75">
+    <row r="41" spans="1:4" ht="30.75" thickBot="1">
+      <c r="A41" s="53">
         <v>38</v>
       </c>
-      <c r="B41" s="76" t="s">
+      <c r="B41" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="76"/>
-      <c r="D41" s="76">
+      <c r="C41" s="54">
         <v>6</v>
       </c>
-      <c r="E41" s="76" t="s">
+      <c r="D41" s="54" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A42" s="75">
+    <row r="42" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A42" s="53">
         <v>39</v>
       </c>
-      <c r="B42" s="76" t="s">
+      <c r="B42" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="76"/>
-      <c r="D42" s="76">
+      <c r="C42" s="54">
         <v>6</v>
       </c>
-      <c r="E42" s="76" t="s">
+      <c r="D42" s="54" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A43" s="75">
+    <row r="43" spans="1:4" ht="30.75" thickBot="1">
+      <c r="A43" s="53">
         <v>40</v>
       </c>
-      <c r="B43" s="76" t="s">
+      <c r="B43" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="76"/>
-      <c r="D43" s="76">
+      <c r="C43" s="54">
         <v>10</v>
       </c>
-      <c r="E43" s="76" t="s">
+      <c r="D43" s="54" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="30.75" thickBot="1">
+    <row r="44" spans="1:4" ht="30.75" thickBot="1">
       <c r="A44" s="35">
         <v>41</v>
       </c>
       <c r="B44" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36">
+      <c r="C44" s="36">
         <v>2</v>
       </c>
-      <c r="E44" s="36" t="s">
+      <c r="D44" s="36" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A45" s="75">
+    <row r="45" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A45" s="53">
         <v>42</v>
       </c>
-      <c r="B45" s="76" t="s">
+      <c r="B45" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="76"/>
-      <c r="D45" s="76">
+      <c r="C45" s="54">
         <v>5</v>
       </c>
-      <c r="E45" s="76" t="s">
+      <c r="D45" s="54" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" thickBot="1">
+    <row r="46" spans="1:4" ht="15.75" thickBot="1">
       <c r="A46" s="35">
         <v>43</v>
       </c>
       <c r="B46" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36">
+      <c r="C46" s="36">
         <v>4</v>
       </c>
-      <c r="E46" s="36" t="s">
+      <c r="D46" s="36" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" thickBot="1">
+    <row r="47" spans="1:4" ht="15.75" thickBot="1">
       <c r="A47" s="35">
         <v>44</v>
       </c>
       <c r="B47" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36">
+      <c r="C47" s="36">
         <v>3</v>
       </c>
-      <c r="E47" s="36" t="s">
+      <c r="D47" s="36" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" thickBot="1">
+    <row r="48" spans="1:4" ht="15.75" thickBot="1">
       <c r="A48" s="35">
         <v>45</v>
       </c>
       <c r="B48" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="C48" s="36"/>
-      <c r="D48" s="36">
+      <c r="C48" s="36">
         <v>6</v>
       </c>
-      <c r="E48" s="36" t="s">
+      <c r="D48" s="36" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.75" thickBot="1">
+    <row r="49" spans="1:4" ht="15.75" thickBot="1">
       <c r="A49" s="35">
         <v>46</v>
       </c>
       <c r="B49" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36">
+      <c r="C49" s="36">
         <v>3</v>
       </c>
-      <c r="E49" s="36" t="s">
+      <c r="D49" s="36" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="30.75" thickBot="1">
+    <row r="50" spans="1:4" ht="30.75" thickBot="1">
       <c r="A50" s="41">
         <v>47</v>
       </c>
       <c r="B50" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="C50" s="42"/>
-      <c r="D50" s="42">
+      <c r="C50" s="42">
         <v>3</v>
       </c>
-      <c r="E50" s="42" t="s">
+      <c r="D50" s="42" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A51" s="75">
+    <row r="51" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A51" s="53">
         <v>48</v>
       </c>
-      <c r="B51" s="79" t="s">
+      <c r="B51" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="C51" s="80"/>
-      <c r="D51" s="80">
+      <c r="C51" s="58">
         <v>13</v>
       </c>
-      <c r="E51" s="81" t="s">
+      <c r="D51" s="59" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.75" thickBot="1">
+    <row r="52" spans="1:4" ht="15.75" thickBot="1">
       <c r="A52" s="35">
         <v>49</v>
       </c>
       <c r="B52" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="C52" s="28"/>
-      <c r="D52" s="28">
-        <f>SUM(D3:D51)</f>
+      <c r="C52" s="28">
+        <f>SUM(C3:C51)</f>
         <v>435</v>
       </c>
-      <c r="E52" s="28"/>
-    </row>
-    <row r="53" spans="1:5" ht="15.75" thickBot="1">
+      <c r="D52" s="28"/>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" thickBot="1">
       <c r="A53" s="35">
         <v>50</v>
       </c>
@@ -2126,12 +2071,11 @@
         <v>81</v>
       </c>
       <c r="C53" s="36"/>
-      <c r="D53" s="36"/>
-      <c r="E53" s="36" t="s">
+      <c r="D53" s="36" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15.75" thickBot="1">
+    <row r="54" spans="1:4" ht="15.75" thickBot="1">
       <c r="A54" s="35">
         <v>51</v>
       </c>
@@ -2140,61 +2084,56 @@
       </c>
       <c r="C54" s="36"/>
       <c r="D54" s="36"/>
-      <c r="E54" s="36"/>
-    </row>
-    <row r="55" spans="1:5" ht="15.75" thickBot="1">
+    </row>
+    <row r="55" spans="1:4" ht="15.75" thickBot="1">
       <c r="A55" s="35">
         <v>52</v>
       </c>
       <c r="B55" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="C55" s="36"/>
-      <c r="D55" s="36">
+      <c r="C55" s="36">
         <v>10</v>
       </c>
-      <c r="E55" s="36"/>
-    </row>
-    <row r="56" spans="1:5" ht="30.75" thickBot="1">
+      <c r="D55" s="36"/>
+    </row>
+    <row r="56" spans="1:4" ht="30.75" thickBot="1">
       <c r="A56" s="35">
         <v>53</v>
       </c>
       <c r="B56" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36">
+      <c r="C56" s="36">
         <v>48</v>
       </c>
-      <c r="E56" s="36" t="s">
+      <c r="D56" s="36" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15.75" thickBot="1">
+    <row r="57" spans="1:4" ht="15.75" thickBot="1">
       <c r="A57" s="35">
         <v>54</v>
       </c>
       <c r="B57" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C57" s="36"/>
-      <c r="D57" s="36">
+      <c r="C57" s="36">
         <v>3</v>
       </c>
-      <c r="E57" s="36" t="s">
+      <c r="D57" s="36" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:4">
       <c r="A58" s="28"/>
       <c r="B58" s="28"/>
       <c r="C58" s="28"/>
       <c r="D58" s="28"/>
-      <c r="E58" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2205,7 +2144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
@@ -2221,15 +2160,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="51"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="62"/>
     </row>
     <row r="2" spans="1:7" ht="30.75" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -2409,17 +2348,17 @@
       <c r="A11" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="62"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="65"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="66" t="s">
         <v>133</v>
       </c>
       <c r="B12" s="3">
@@ -2440,7 +2379,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A13" s="63"/>
+      <c r="A13" s="67"/>
       <c r="B13" s="3">
         <v>8</v>
       </c>
@@ -2459,7 +2398,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A14" s="63"/>
+      <c r="A14" s="67"/>
       <c r="B14" s="3">
         <v>9</v>
       </c>
@@ -2478,7 +2417,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A15" s="63"/>
+      <c r="A15" s="67"/>
       <c r="B15" s="3">
         <v>10</v>
       </c>
@@ -2497,7 +2436,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A16" s="63"/>
+      <c r="A16" s="67"/>
       <c r="B16" s="3">
         <v>11</v>
       </c>
@@ -2516,7 +2455,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="30.75" thickBot="1">
-      <c r="A17" s="63"/>
+      <c r="A17" s="67"/>
       <c r="B17" s="9">
         <v>12</v>
       </c>
@@ -2535,7 +2474,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A18" s="63"/>
+      <c r="A18" s="67"/>
       <c r="B18" s="9">
         <v>13</v>
       </c>
@@ -2554,7 +2493,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="30.75" thickBot="1">
-      <c r="A19" s="63"/>
+      <c r="A19" s="67"/>
       <c r="B19" s="9">
         <v>14</v>
       </c>
@@ -2573,7 +2512,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="30">
-      <c r="A20" s="63"/>
+      <c r="A20" s="67"/>
       <c r="B20" s="18">
         <v>15</v>
       </c>
@@ -2592,7 +2531,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="30">
-      <c r="A21" s="63"/>
+      <c r="A21" s="67"/>
       <c r="B21" s="19"/>
       <c r="C21" s="32" t="s">
         <v>114</v>
@@ -2609,7 +2548,7 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="63"/>
+      <c r="A22" s="67"/>
       <c r="B22" s="29">
         <v>16</v>
       </c>
@@ -2628,7 +2567,7 @@
       <c r="I22" s="21"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="64"/>
+      <c r="A23" s="68"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
       <c r="D23" s="20">
@@ -2643,17 +2582,17 @@
       <c r="A24" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="65" t="s">
+      <c r="B24" s="69" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="66"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="68"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="72"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A25" s="52" t="s">
+      <c r="A25" s="66" t="s">
         <v>134</v>
       </c>
       <c r="B25" s="35">
@@ -2674,7 +2613,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A26" s="53"/>
+      <c r="A26" s="73"/>
       <c r="B26" s="35">
         <v>18</v>
       </c>
@@ -2693,7 +2632,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A27" s="53"/>
+      <c r="A27" s="73"/>
       <c r="B27" s="35">
         <v>19</v>
       </c>
@@ -2712,7 +2651,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A28" s="53"/>
+      <c r="A28" s="73"/>
       <c r="B28" s="35">
         <v>20</v>
       </c>
@@ -2731,7 +2670,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="30">
-      <c r="A29" s="53"/>
+      <c r="A29" s="73"/>
       <c r="B29" s="30">
         <v>15</v>
       </c>
@@ -2750,7 +2689,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A30" s="53"/>
+      <c r="A30" s="73"/>
       <c r="B30" s="35">
         <v>21</v>
       </c>
@@ -2769,7 +2708,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A31" s="53"/>
+      <c r="A31" s="73"/>
       <c r="B31" s="35">
         <v>23</v>
       </c>
@@ -2788,7 +2727,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A32" s="53"/>
+      <c r="A32" s="73"/>
       <c r="B32" s="35">
         <v>24</v>
       </c>
@@ -2807,7 +2746,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A33" s="53"/>
+      <c r="A33" s="73"/>
       <c r="B33" s="35">
         <v>28</v>
       </c>
@@ -2826,13 +2765,13 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="53"/>
+      <c r="A34" s="73"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="53"/>
+      <c r="A35" s="73"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A36" s="53"/>
+      <c r="A36" s="73"/>
       <c r="D36">
         <f>SUM(D25:D33)</f>
         <v>80</v>
@@ -2840,29 +2779,29 @@
       <c r="G36" s="36"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A37" s="54"/>
-      <c r="B37" s="55"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="57"/>
+      <c r="A37" s="74"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="76"/>
+      <c r="F37" s="76"/>
+      <c r="G37" s="77"/>
     </row>
     <row r="38" spans="1:7" ht="29.25" thickBot="1">
       <c r="A38" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B38" s="58" t="s">
+      <c r="B38" s="78" t="s">
         <v>125</v>
       </c>
-      <c r="C38" s="59"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="59"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="79"/>
+      <c r="E38" s="79"/>
+      <c r="F38" s="79"/>
+      <c r="G38" s="79"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A39" s="52" t="s">
+      <c r="A39" s="66" t="s">
         <v>135</v>
       </c>
       <c r="B39" s="35">
@@ -2883,7 +2822,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A40" s="53"/>
+      <c r="A40" s="73"/>
       <c r="B40" s="35">
         <v>26</v>
       </c>
@@ -2902,7 +2841,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A41" s="53"/>
+      <c r="A41" s="73"/>
       <c r="B41" s="35">
         <v>30</v>
       </c>
@@ -2920,7 +2859,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A42" s="53"/>
+      <c r="A42" s="73"/>
       <c r="B42" s="35">
         <v>31</v>
       </c>
@@ -2938,7 +2877,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A43" s="53"/>
+      <c r="A43" s="73"/>
       <c r="B43" s="35">
         <v>33</v>
       </c>
@@ -2956,7 +2895,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A44" s="53"/>
+      <c r="A44" s="73"/>
       <c r="B44" s="35">
         <v>35</v>
       </c>
@@ -2974,7 +2913,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A45" s="53"/>
+      <c r="A45" s="73"/>
       <c r="B45" s="35">
         <v>36</v>
       </c>
@@ -2992,7 +2931,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A46" s="53"/>
+      <c r="A46" s="73"/>
       <c r="B46" s="35">
         <v>34</v>
       </c>
@@ -3011,7 +2950,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A47" s="53"/>
+      <c r="A47" s="73"/>
       <c r="B47" s="35"/>
       <c r="C47" s="34"/>
       <c r="D47" s="34">
@@ -3020,39 +2959,39 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A48" s="53"/>
+      <c r="A48" s="73"/>
       <c r="B48" s="35"/>
       <c r="C48" s="34"/>
       <c r="D48" s="34"/>
     </row>
     <row r="49" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A49" s="53"/>
+      <c r="A49" s="73"/>
       <c r="G49" s="36"/>
     </row>
     <row r="50" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A50" s="54"/>
-      <c r="B50" s="55"/>
-      <c r="C50" s="56"/>
-      <c r="D50" s="56"/>
-      <c r="E50" s="56"/>
-      <c r="F50" s="56"/>
-      <c r="G50" s="57"/>
+      <c r="A50" s="74"/>
+      <c r="B50" s="75"/>
+      <c r="C50" s="76"/>
+      <c r="D50" s="76"/>
+      <c r="E50" s="76"/>
+      <c r="F50" s="76"/>
+      <c r="G50" s="77"/>
     </row>
     <row r="51" spans="1:7" ht="29.25" thickBot="1">
       <c r="A51" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B51" s="58" t="s">
+      <c r="B51" s="78" t="s">
         <v>125</v>
       </c>
-      <c r="C51" s="59"/>
-      <c r="D51" s="59"/>
-      <c r="E51" s="59"/>
-      <c r="F51" s="59"/>
-      <c r="G51" s="59"/>
+      <c r="C51" s="79"/>
+      <c r="D51" s="79"/>
+      <c r="E51" s="79"/>
+      <c r="F51" s="79"/>
+      <c r="G51" s="79"/>
     </row>
     <row r="52" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A52" s="52" t="s">
+      <c r="A52" s="66" t="s">
         <v>136</v>
       </c>
       <c r="B52" s="35">
@@ -3071,7 +3010,7 @@
       <c r="G52" s="29"/>
     </row>
     <row r="53" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A53" s="53"/>
+      <c r="A53" s="73"/>
       <c r="B53" s="35">
         <v>32</v>
       </c>
@@ -3088,7 +3027,7 @@
       <c r="G53" s="29"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A54" s="53"/>
+      <c r="A54" s="73"/>
       <c r="B54" s="35">
         <v>48</v>
       </c>
@@ -3104,7 +3043,7 @@
       <c r="G54" s="29"/>
     </row>
     <row r="55" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A55" s="53"/>
+      <c r="A55" s="73"/>
       <c r="B55" s="35">
         <v>42</v>
       </c>
@@ -3120,7 +3059,7 @@
       <c r="G55" s="29"/>
     </row>
     <row r="56" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A56" s="53"/>
+      <c r="A56" s="73"/>
       <c r="B56" s="35">
         <v>37</v>
       </c>
@@ -3136,7 +3075,7 @@
       <c r="G56" s="29"/>
     </row>
     <row r="57" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A57" s="53"/>
+      <c r="A57" s="73"/>
       <c r="B57" s="35">
         <v>38</v>
       </c>
@@ -3152,7 +3091,7 @@
       <c r="G57" s="29"/>
     </row>
     <row r="58" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A58" s="53"/>
+      <c r="A58" s="73"/>
       <c r="B58" s="35">
         <v>39</v>
       </c>
@@ -3168,7 +3107,7 @@
       <c r="G58" s="29"/>
     </row>
     <row r="59" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A59" s="53"/>
+      <c r="A59" s="73"/>
       <c r="B59" s="35">
         <v>40</v>
       </c>
@@ -3185,7 +3124,7 @@
       <c r="G59" s="29"/>
     </row>
     <row r="60" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A60" s="53"/>
+      <c r="A60" s="73"/>
       <c r="B60" s="35"/>
       <c r="C60" s="34"/>
       <c r="D60" s="34">
@@ -3194,23 +3133,23 @@
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A61" s="53"/>
+      <c r="A61" s="73"/>
       <c r="B61" s="35"/>
       <c r="C61" s="34"/>
       <c r="D61" s="34"/>
     </row>
     <row r="62" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A62" s="53"/>
+      <c r="A62" s="73"/>
       <c r="G62" s="36"/>
     </row>
     <row r="63" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A63" s="54"/>
-      <c r="B63" s="55"/>
-      <c r="C63" s="56"/>
-      <c r="D63" s="56"/>
-      <c r="E63" s="56"/>
-      <c r="F63" s="56"/>
-      <c r="G63" s="57"/>
+      <c r="A63" s="74"/>
+      <c r="B63" s="75"/>
+      <c r="C63" s="76"/>
+      <c r="D63" s="76"/>
+      <c r="E63" s="76"/>
+      <c r="F63" s="76"/>
+      <c r="G63" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3249,12 +3188,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24" thickBot="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
     </row>
     <row r="2" spans="1:4" ht="20.25" thickBot="1">
       <c r="A2" s="12" t="s">
@@ -3302,13 +3241,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="51"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="62"/>
     </row>
     <row r="2" spans="1:5" ht="30">
       <c r="A2" s="22" t="s">

</xml_diff>

<commit_message>
CAPITULO 3-ANALISIS Y EVALUACION DE TECNOLOGIAS DE REALIDAD AUMENTADA..docx actualizacion
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="130">
   <si>
     <t>Product Backlog Items-Prototipo de Realidad Aumentada</t>
   </si>
@@ -2078,8 +2078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:G16"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2882,7 +2882,9 @@
       <c r="F49" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="G49" s="28"/>
+      <c r="G49" s="28" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" thickBot="1">
       <c r="A50" s="72"/>
@@ -2899,7 +2901,9 @@
       <c r="F50" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="G50" s="28"/>
+      <c r="G50" s="28" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" thickBot="1">
       <c r="A51" s="72"/>
@@ -2963,7 +2967,9 @@
       <c r="F54" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="G54" s="28"/>
+      <c r="G54" s="28" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" thickBot="1">
       <c r="A55" s="72"/>

</xml_diff>

<commit_message>
Desarrollo de inferza-grupo diseño.docx agragado de imagenes
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="133">
   <si>
     <t>Product Backlog Items-Prototipo de Realidad Aumentada</t>
   </si>
@@ -408,6 +408,15 @@
   </si>
   <si>
     <t>Sprint 05 2/07/14 - 31/07/14</t>
+  </si>
+  <si>
+    <t>Coordinar con las chicas la interfaz del sistema.</t>
+  </si>
+  <si>
+    <t>Realizar entrevistas con pablo</t>
+  </si>
+  <si>
+    <t>El icono, el splash, botones nevegacion, box de pedido(about)</t>
   </si>
 </sst>
 </file>
@@ -1314,10 +1323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:D14"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1325,7 +1334,7 @@
     <col min="1" max="1" width="5.85546875" customWidth="1"/>
     <col min="2" max="2" width="40.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="47.42578125" customWidth="1"/>
+    <col min="4" max="4" width="69" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1">
@@ -2060,10 +2069,23 @@
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="27"/>
+      <c r="A55" s="29"/>
       <c r="B55" s="27"/>
       <c r="C55" s="27"/>
       <c r="D55" s="27"/>
+    </row>
+    <row r="56" spans="1:4" ht="30">
+      <c r="B56" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="D56" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="B57" s="36" t="s">
+        <v>131</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2078,8 +2100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Casos de prueba y tareas que faltan hacer scrum.xlsx
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="139">
   <si>
     <t>Product Backlog Items-Prototipo de Realidad Aumentada</t>
   </si>
@@ -417,6 +417,24 @@
   </si>
   <si>
     <t>Realizar entrevistas con pablo primer encuentro</t>
+  </si>
+  <si>
+    <t>Realizar entrevistas con pablo segundi encuentro</t>
+  </si>
+  <si>
+    <t>Arreglar el login-el passwor no debe verse.</t>
+  </si>
+  <si>
+    <t>Arreglar pantalla de login incorrecto</t>
+  </si>
+  <si>
+    <t>Ver el tema de las empanadas, agregar cantidad</t>
+  </si>
+  <si>
+    <t>Cambiar para el el pdf se guarde en mis documentos, mis documentos siempre va existir</t>
+  </si>
+  <si>
+    <t>Faltan dos casos de uso agregar diario y elimiar</t>
   </si>
 </sst>
 </file>
@@ -1323,10 +1341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2085,6 +2103,36 @@
     <row r="57" spans="1:4" ht="30">
       <c r="B57" s="36" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="B58" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="B59" s="36" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="B60" s="36" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="30">
+      <c r="B61" s="36" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="45">
+      <c r="B62" s="36" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="30">
+      <c r="B63" s="36" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Casos de prueba  y agregado de tareas
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="141">
   <si>
     <t>Product Backlog Items-Prototipo de Realidad Aumentada</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>Cambiar la descripcion de la tabla de menu en la base de datos, solo aparece descripcion</t>
+  </si>
+  <si>
+    <t>Cambiar el nombre de la tabla TEA_MENU_PEDIDO por DETALLE_PEDIDO (ya lo cambie en los casos de prueba)</t>
   </si>
 </sst>
 </file>
@@ -1344,16 +1347,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="69" customWidth="1"/>
   </cols>
@@ -2141,6 +2144,11 @@
     <row r="64" spans="1:4" ht="45">
       <c r="B64" s="36" t="s">
         <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" ht="30">
+      <c r="B65" s="36" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregado de tareas extras
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="143">
   <si>
     <t>Product Backlog Items-Prototipo de Realidad Aumentada</t>
   </si>
@@ -441,6 +441,12 @@
   </si>
   <si>
     <t>Cambiar el nombre de la tabla TEA_MENU_PEDIDO por DETALLE_PEDIDO (ya lo cambie en los casos de prueba)</t>
+  </si>
+  <si>
+    <t>Resolver el numero de ip para android</t>
+  </si>
+  <si>
+    <t>Crear la interfaz para ingresar ip de servidor</t>
   </si>
 </sst>
 </file>
@@ -1347,10 +1353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1397,7 +1403,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45.75" thickBot="1">
+    <row r="4" spans="1:4" ht="30.75" thickBot="1">
       <c r="A4" s="38">
         <v>1</v>
       </c>
@@ -1425,7 +1431,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30.75" thickBot="1">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1">
       <c r="A6" s="38">
         <v>4</v>
       </c>
@@ -1613,7 +1619,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30.75" thickBot="1">
+    <row r="20" spans="1:6" ht="15.75" thickBot="1">
       <c r="A20" s="42">
         <v>19</v>
       </c>
@@ -1919,7 +1925,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30.75" thickBot="1">
+    <row r="42" spans="1:4" ht="15.75" thickBot="1">
       <c r="A42" s="52">
         <v>42</v>
       </c>
@@ -2098,7 +2104,7 @@
       <c r="C55" s="27"/>
       <c r="D55" s="27"/>
     </row>
-    <row r="56" spans="1:4" ht="30">
+    <row r="56" spans="1:4">
       <c r="B56" s="36" t="s">
         <v>130</v>
       </c>
@@ -2106,7 +2112,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="30">
+    <row r="57" spans="1:4">
       <c r="B57" s="36" t="s">
         <v>132</v>
       </c>
@@ -2126,22 +2132,22 @@
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="30">
+    <row r="61" spans="1:4">
       <c r="B61" s="36" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="45">
+    <row r="62" spans="1:4" ht="30">
       <c r="B62" s="36" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="30">
+    <row r="63" spans="1:4">
       <c r="B63" s="36" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="45">
+    <row r="64" spans="1:4" ht="30">
       <c r="B64" s="36" t="s">
         <v>139</v>
       </c>
@@ -2149,6 +2155,16 @@
     <row r="65" spans="2:2" ht="30">
       <c r="B65" s="36" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" s="36" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion de product backlog
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="142">
   <si>
     <t>Product Backlog Items-Prototipo de Realidad Aumentada</t>
   </si>
@@ -441,9 +441,6 @@
   </si>
   <si>
     <t>Cambiar el nombre de la tabla TEA_MENU_PEDIDO por DETALLE_PEDIDO (ya lo cambie en los casos de prueba)</t>
-  </si>
-  <si>
-    <t>Resolver el numero de ip para android</t>
   </si>
   <si>
     <t>Crear la interfaz para ingresar ip de servidor</t>
@@ -1353,10 +1350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2160,11 +2157,6 @@
     <row r="66" spans="2:2">
       <c r="B66" s="36" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2">
-      <c r="B67" s="36" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Casos de prueba.docx finalizados y mas tareas para hacer en scrum.xlsx
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="143">
   <si>
     <t>Product Backlog Items-Prototipo de Realidad Aumentada</t>
   </si>
@@ -440,10 +440,13 @@
     <t>Cambiar la descripcion de la tabla de menu en la base de datos, solo aparece descripcion</t>
   </si>
   <si>
-    <t>Cambiar el nombre de la tabla TEA_MENU_PEDIDO por DETALLE_PEDIDO (ya lo cambie en los casos de prueba)</t>
-  </si>
-  <si>
     <t>Crear la interfaz para ingresar ip de servidor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cambiar el nombre de la tabla TEA_MENU_PEDIDO por DETALLE_PEDIDO (ya lo cambie en los casos de prueba) , en la base de datos debe quedar:  DET_PED_ID; DET_PED _CANTIDAD y DET_PED _ESTADO </t>
+  </si>
+  <si>
+    <t>Fijarse en la pantalla de pedido y editar el nombre idPedio por id</t>
   </si>
 </sst>
 </file>
@@ -1350,10 +1353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2149,14 +2152,19 @@
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="2:2" ht="30">
+    <row r="65" spans="2:2" ht="60">
       <c r="B65" s="36" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" s="36" t="s">
-        <v>141</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" ht="30">
+      <c r="B67" s="36" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregadas tareas al scrum.xlsx
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="148">
   <si>
     <t>Product Backlog Items-Prototipo de Realidad Aumentada</t>
   </si>
@@ -447,6 +447,21 @@
   </si>
   <si>
     <t>Fijarse en la pantalla de pedido y editar el nombre idPedio por id</t>
+  </si>
+  <si>
+    <t>hecho</t>
+  </si>
+  <si>
+    <t>hecha</t>
+  </si>
+  <si>
+    <t>leer marco teorico</t>
+  </si>
+  <si>
+    <t>cambiar el doc de preparacion de entorno de trabajo CP5</t>
+  </si>
+  <si>
+    <t>acomodar las interfaz de de escritotio</t>
   </si>
 </sst>
 </file>
@@ -1353,10 +1368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView topLeftCell="A56" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2023,7 +2038,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" thickBot="1">
+    <row r="49" spans="1:5" ht="15.75" thickBot="1">
       <c r="A49" s="34">
         <v>49</v>
       </c>
@@ -2036,7 +2051,7 @@
       </c>
       <c r="D49" s="27"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" thickBot="1">
+    <row r="50" spans="1:5" ht="15.75" thickBot="1">
       <c r="A50" s="34">
         <v>50</v>
       </c>
@@ -2048,7 +2063,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75" thickBot="1">
+    <row r="51" spans="1:5" ht="15.75" thickBot="1">
       <c r="A51" s="34">
         <v>51</v>
       </c>
@@ -2058,7 +2073,7 @@
       <c r="C51" s="35"/>
       <c r="D51" s="35"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75" thickBot="1">
+    <row r="52" spans="1:5" ht="15.75" thickBot="1">
       <c r="A52" s="34">
         <v>52</v>
       </c>
@@ -2070,7 +2085,7 @@
       </c>
       <c r="D52" s="35"/>
     </row>
-    <row r="53" spans="1:4" ht="30.75" thickBot="1">
+    <row r="53" spans="1:5" ht="30.75" thickBot="1">
       <c r="A53" s="34">
         <v>53</v>
       </c>
@@ -2084,7 +2099,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="30.75" thickBot="1">
+    <row r="54" spans="1:5" ht="30.75" thickBot="1">
       <c r="A54" s="34">
         <v>54</v>
       </c>
@@ -2098,13 +2113,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:5">
       <c r="A55" s="29"/>
       <c r="B55" s="27"/>
       <c r="C55" s="27"/>
       <c r="D55" s="27"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:5">
       <c r="B56" s="36" t="s">
         <v>130</v>
       </c>
@@ -2112,59 +2127,86 @@
         <v>131</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:5">
       <c r="B57" s="36" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="B58" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:5">
       <c r="B59" s="36" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="E59" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="B60" s="36" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:5">
       <c r="B61" s="36" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="30">
+    <row r="62" spans="1:5" ht="30">
       <c r="B62" s="36" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:5">
       <c r="B63" s="36" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="30">
+      <c r="E63" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="30">
       <c r="B64" s="36" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="2:2" ht="60">
+    <row r="65" spans="2:5" ht="60">
       <c r="B65" s="36" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="66" spans="2:2">
+      <c r="E65" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5">
       <c r="B66" s="36" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="67" spans="2:2" ht="30">
+    <row r="67" spans="2:5" ht="30">
       <c r="B67" s="36" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5">
+      <c r="B69" s="36" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5">
+      <c r="B70" s="36" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5">
+      <c r="B71" s="36" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2180,7 +2222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
       <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
agregadas tareas a scrum
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="149">
   <si>
     <t>Product Backlog Items-Prototipo de Realidad Aumentada</t>
   </si>
@@ -1373,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2102,7 +2102,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="30.75" thickBot="1">
+    <row r="54" spans="1:5" ht="15.75" thickBot="1">
       <c r="A54" s="34">
         <v>54</v>
       </c>
@@ -2202,6 +2202,9 @@
     </row>
     <row r="69" spans="2:5">
       <c r="B69" s="36"/>
+      <c r="E69" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="70" spans="2:5">
       <c r="B70" s="36" t="s">
@@ -2222,6 +2225,9 @@
     <row r="72" spans="2:5" ht="30">
       <c r="B72" s="36" t="s">
         <v>147</v>
+      </c>
+      <c r="E72" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="2:5">

</xml_diff>

<commit_message>
agregadas nuevas tareas al scrum
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="160">
   <si>
     <t>Product Backlog Items-Prototipo de Realidad Aumentada</t>
   </si>
@@ -471,6 +471,33 @@
   </si>
   <si>
     <t>pend</t>
+  </si>
+  <si>
+    <t>investigar incrutacion de video</t>
+  </si>
+  <si>
+    <t>acomodar apk</t>
+  </si>
+  <si>
+    <t>cortar y listar videos</t>
+  </si>
+  <si>
+    <t>agregar videos al sistema</t>
+  </si>
+  <si>
+    <t>hacer nuevas capturas para la interfaz</t>
+  </si>
+  <si>
+    <t>completar marco teorico con info de discapacitados</t>
+  </si>
+  <si>
+    <t>terminar conclusion y  lineas futuras</t>
+  </si>
+  <si>
+    <t>hacer manual de usuario</t>
+  </si>
+  <si>
+    <t>revision total final de la documentacion</t>
   </si>
 </sst>
 </file>
@@ -1377,10 +1404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2151,8 +2178,8 @@
       <c r="B58" t="s">
         <v>133</v>
       </c>
-      <c r="F58" t="s">
-        <v>150</v>
+      <c r="E58" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2263,7 +2290,49 @@
       </c>
     </row>
     <row r="74" spans="2:5">
-      <c r="B74" s="36"/>
+      <c r="B74" s="36" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5">
+      <c r="B75" s="36" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5">
+      <c r="B76" s="36" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5">
+      <c r="B77" s="36" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5">
+      <c r="B78" s="36" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5">
+      <c r="B79" s="36" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5">
+      <c r="B80" s="36" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" s="36" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2">
+      <c r="B82" s="36" t="s">
+        <v>159</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
nuevas tareas al scrum
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="162">
   <si>
     <t>Product Backlog Items-Prototipo de Realidad Aumentada</t>
   </si>
@@ -498,6 +498,12 @@
   </si>
   <si>
     <t>revision total final de la documentacion</t>
+  </si>
+  <si>
+    <t>investigar como genera exe con VS</t>
+  </si>
+  <si>
+    <t>dar formato final de a los documetnos</t>
   </si>
 </sst>
 </file>
@@ -1404,10 +1410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2321,16 +2327,26 @@
     </row>
     <row r="80" spans="2:5">
       <c r="B80" s="36" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="81" spans="2:2">
       <c r="B81" s="36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="82" spans="2:2">
       <c r="B82" s="36" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" s="36" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84" s="36" t="s">
         <v>159</v>
       </c>
     </row>

</xml_diff>

<commit_message>
arreglo de fechas e el sistema
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="164">
   <si>
     <t>Product Backlog Items-Prototipo de Realidad Aumentada</t>
   </si>
@@ -1418,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="C65" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2242,7 +2242,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="65" spans="2:5" ht="60">
+    <row r="65" spans="2:6" ht="60">
       <c r="B65" s="36" t="s">
         <v>140</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="66" spans="2:5">
+    <row r="66" spans="2:6">
       <c r="B66" s="36" t="s">
         <v>139</v>
       </c>
@@ -2258,23 +2258,29 @@
         <v>148</v>
       </c>
     </row>
-    <row r="67" spans="2:5" ht="30">
+    <row r="67" spans="2:6" ht="30">
       <c r="B67" s="36" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="68" spans="2:5">
+    <row r="68" spans="2:6">
       <c r="B68" s="36" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="69" spans="2:5">
+      <c r="E68" t="s">
+        <v>143</v>
+      </c>
+      <c r="F68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6">
       <c r="B69" s="36"/>
       <c r="E69" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="70" spans="2:5">
+    <row r="70" spans="2:6">
       <c r="B70" s="36" t="s">
         <v>147</v>
       </c>
@@ -2285,7 +2291,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="71" spans="2:5">
+    <row r="71" spans="2:6">
       <c r="B71" s="36" t="s">
         <v>144</v>
       </c>
@@ -2293,7 +2299,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="72" spans="2:5" ht="30">
+    <row r="72" spans="2:6" ht="30">
       <c r="B72" s="36" t="s">
         <v>146</v>
       </c>
@@ -2301,12 +2307,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="73" spans="2:5">
+    <row r="73" spans="2:6">
       <c r="B73" s="36" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="74" spans="2:5">
+    <row r="74" spans="2:6">
       <c r="B74" s="36" t="s">
         <v>151</v>
       </c>
@@ -2314,7 +2320,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="75" spans="2:5">
+    <row r="75" spans="2:6">
       <c r="B75" s="36" t="s">
         <v>152</v>
       </c>
@@ -2322,7 +2328,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="76" spans="2:5">
+    <row r="76" spans="2:6">
       <c r="B76" s="36" t="s">
         <v>153</v>
       </c>
@@ -2330,22 +2336,22 @@
         <v>143</v>
       </c>
     </row>
-    <row r="77" spans="2:5">
+    <row r="77" spans="2:6">
       <c r="B77" s="36" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="78" spans="2:5">
+    <row r="78" spans="2:6">
       <c r="B78" s="36" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="79" spans="2:5">
+    <row r="79" spans="2:6">
       <c r="B79" s="36" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="80" spans="2:5">
+    <row r="80" spans="2:6">
       <c r="B80" s="36" t="s">
         <v>156</v>
       </c>

</xml_diff>

<commit_message>
agregado de tareas pendientes
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="167">
   <si>
     <t>Product Backlog Items-Prototipo de Realidad Aumentada</t>
   </si>
@@ -470,9 +470,6 @@
     <t>Cambiar para el el pdf se guarde en el directorio CharlottePedidos, si no exite la crea</t>
   </si>
   <si>
-    <t>pend</t>
-  </si>
-  <si>
     <t>investigar incrutacion de video</t>
   </si>
   <si>
@@ -510,6 +507,18 @@
   </si>
   <si>
     <t>arreglar error en busquedas por fechas</t>
+  </si>
+  <si>
+    <t>correccion de sistema: presionar al boton agregar y que cuadno coicida con el video, no debe reproducirse. Superposicion de botones</t>
+  </si>
+  <si>
+    <t>Reproducirse automaticamente</t>
+  </si>
+  <si>
+    <t>corregir los defectos cuando se reproduce, la interfaz de navegacion se distorsiona</t>
+  </si>
+  <si>
+    <t>Cambiar la extension de los videos a m4v(reconvertir con alguna herramienta)</t>
   </si>
 </sst>
 </file>
@@ -1416,10 +1425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2174,6 +2183,9 @@
       <c r="D56" t="s">
         <v>131</v>
       </c>
+      <c r="E56" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="57" spans="1:6">
       <c r="B57" s="36" t="s">
@@ -2214,8 +2226,8 @@
       <c r="B61" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="F61" t="s">
-        <v>150</v>
+      <c r="E61" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="30">
@@ -2265,7 +2277,7 @@
     </row>
     <row r="68" spans="2:6">
       <c r="B68" s="36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E68" t="s">
         <v>143</v>
@@ -2314,7 +2326,7 @@
     </row>
     <row r="74" spans="2:6">
       <c r="B74" s="36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E74" t="s">
         <v>148</v>
@@ -2322,7 +2334,7 @@
     </row>
     <row r="75" spans="2:6">
       <c r="B75" s="36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E75" t="s">
         <v>148</v>
@@ -2330,7 +2342,7 @@
     </row>
     <row r="76" spans="2:6">
       <c r="B76" s="36" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E76" t="s">
         <v>143</v>
@@ -2338,22 +2350,22 @@
     </row>
     <row r="77" spans="2:6">
       <c r="B77" s="36" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="78" spans="2:6">
       <c r="B78" s="36" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="79" spans="2:6">
       <c r="B79" s="36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="2:6">
       <c r="B80" s="36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E80" t="s">
         <v>143</v>
@@ -2361,7 +2373,7 @@
     </row>
     <row r="81" spans="2:5">
       <c r="B81" s="36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E81" t="s">
         <v>143</v>
@@ -2369,22 +2381,42 @@
     </row>
     <row r="82" spans="2:5">
       <c r="B82" s="36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="83" spans="2:5">
       <c r="B83" s="36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84" spans="2:5">
       <c r="B84" s="36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="85" spans="2:5">
       <c r="B85" s="36" t="s">
-        <v>159</v>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" ht="45">
+      <c r="B86" s="36" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5">
+      <c r="B87" s="36" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" ht="30">
+      <c r="B88" s="36" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" ht="30">
+      <c r="B89" s="36" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>